<commit_message>
closes #36, but differently from #74
</commit_message>
<xml_diff>
--- a/classification-systems/nzlum/build/commodities.xlsx
+++ b/classification-systems/nzlum/build/commodities.xlsx
@@ -484,12 +484,16 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>cattle</t>
+          <t>sheep meat</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr"/>
       <c r="D2" s="2" t="inlineStr"/>
-      <c r="E2" s="2" t="inlineStr"/>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>Sheep for meat production.</t>
+        </is>
+      </c>
       <c r="F2" s="2" t="inlineStr"/>
     </row>
     <row r="3">
@@ -512,26 +516,30 @@
       <c r="A4" s="2" t="n"/>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>bees</t>
+          <t>sheep stud</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr"/>
       <c r="D4" s="2" t="inlineStr"/>
-      <c r="E4" s="2" t="inlineStr"/>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>Sheep raised for sale as breeding animals.</t>
+        </is>
+      </c>
       <c r="F4" s="2" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n"/>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>sheep meat</t>
+          <t>molluscs</t>
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr"/>
       <c r="D5" s="2" t="inlineStr"/>
       <c r="E5" s="2" t="inlineStr">
         <is>
-          <t>Sheep for meat production.</t>
+          <t>Aquaculture: includes peal oysters, edible oysters, abalone, mussels.</t>
         </is>
       </c>
       <c r="F5" s="2" t="inlineStr"/>
@@ -540,14 +548,14 @@
       <c r="A6" s="2" t="n"/>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>molluscs</t>
+          <t>finfish</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr"/>
       <c r="D6" s="2" t="inlineStr"/>
       <c r="E6" s="2" t="inlineStr">
         <is>
-          <t>Aquaculture: includes peal oysters, edible oysters, abalone, mussels.</t>
+          <t>Aquaculture: tuna, salmon, trout, freshwater species, etc.</t>
         </is>
       </c>
       <c r="F6" s="2" t="inlineStr"/>
@@ -556,62 +564,50 @@
       <c r="A7" s="2" t="n"/>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>cats</t>
+          <t>bees</t>
         </is>
       </c>
       <c r="C7" s="2" t="inlineStr"/>
       <c r="D7" s="2" t="inlineStr"/>
-      <c r="E7" s="2" t="inlineStr">
-        <is>
-          <t>Includes cat breeding, catteries, or areas used for quarantine of cats related to import or export.</t>
-        </is>
-      </c>
+      <c r="E7" s="2" t="inlineStr"/>
       <c r="F7" s="2" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n"/>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>goats dairy</t>
+          <t>deer</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr"/>
       <c r="D8" s="2" t="inlineStr"/>
-      <c r="E8" s="2" t="inlineStr">
-        <is>
-          <t>Goats for milk production.</t>
-        </is>
-      </c>
+      <c r="E8" s="2" t="inlineStr"/>
       <c r="F8" s="2" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n"/>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>sheep</t>
+          <t>cattle</t>
         </is>
       </c>
       <c r="C9" s="2" t="inlineStr"/>
       <c r="D9" s="2" t="inlineStr"/>
-      <c r="E9" s="2" t="inlineStr">
-        <is>
-          <t>Specify meat, dairy, stud or wool where appropriate.</t>
-        </is>
-      </c>
+      <c r="E9" s="2" t="inlineStr"/>
       <c r="F9" s="2" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n"/>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>chickens</t>
+          <t>crustaceans</t>
         </is>
       </c>
       <c r="C10" s="2" t="inlineStr"/>
       <c r="D10" s="2" t="inlineStr"/>
       <c r="E10" s="2" t="inlineStr">
         <is>
-          <t>Poultry farms. Specify whether for eggs or meat where possible.</t>
+          <t>Aquaculture: prawns, freshwater crayfish, etc.</t>
         </is>
       </c>
       <c r="F10" s="2" t="inlineStr"/>
@@ -620,14 +616,14 @@
       <c r="A11" s="2" t="n"/>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>ostriches</t>
+          <t>sheep dairy</t>
         </is>
       </c>
       <c r="C11" s="2" t="inlineStr"/>
       <c r="D11" s="2" t="inlineStr"/>
       <c r="E11" s="2" t="inlineStr">
         <is>
-          <t>Poultry farming.</t>
+          <t>Sheep for milk production.</t>
         </is>
       </c>
       <c r="F11" s="2" t="inlineStr"/>
@@ -636,14 +632,14 @@
       <c r="A12" s="2" t="n"/>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>pigs</t>
+          <t>ostriches</t>
         </is>
       </c>
       <c r="C12" s="2" t="inlineStr"/>
       <c r="D12" s="2" t="inlineStr"/>
       <c r="E12" s="2" t="inlineStr">
         <is>
-          <t>Piggeries.</t>
+          <t>Poultry farming.</t>
         </is>
       </c>
       <c r="F12" s="2" t="inlineStr"/>
@@ -652,14 +648,14 @@
       <c r="A13" s="2" t="n"/>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>dogs</t>
+          <t>cattle meat</t>
         </is>
       </c>
       <c r="C13" s="2" t="inlineStr"/>
       <c r="D13" s="2" t="inlineStr"/>
       <c r="E13" s="2" t="inlineStr">
         <is>
-          <t>Includes dog breeding, kennels, or areas used for quarantine of dogs related to import or export.</t>
+          <t>Cattle for meat (beef) production.</t>
         </is>
       </c>
       <c r="F13" s="2" t="inlineStr"/>
@@ -668,14 +664,14 @@
       <c r="A14" s="2" t="n"/>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>finfish</t>
+          <t>sheep wool</t>
         </is>
       </c>
       <c r="C14" s="2" t="inlineStr"/>
       <c r="D14" s="2" t="inlineStr"/>
       <c r="E14" s="2" t="inlineStr">
         <is>
-          <t>Aquaculture: tuna, salmon, trout, freshwater species, etc.</t>
+          <t>Sheep for fibre production.</t>
         </is>
       </c>
       <c r="F14" s="2" t="inlineStr"/>
@@ -684,14 +680,14 @@
       <c r="A15" s="2" t="n"/>
       <c r="B15" s="2" t="inlineStr">
         <is>
-          <t>crocodiles</t>
+          <t>turkeys</t>
         </is>
       </c>
       <c r="C15" s="2" t="inlineStr"/>
       <c r="D15" s="2" t="inlineStr"/>
       <c r="E15" s="2" t="inlineStr">
         <is>
-          <t>Aquaculture.</t>
+          <t>Poultry farms.</t>
         </is>
       </c>
       <c r="F15" s="2" t="inlineStr"/>
@@ -700,14 +696,14 @@
       <c r="A16" s="2" t="n"/>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>geese</t>
+          <t>chickens eggs</t>
         </is>
       </c>
       <c r="C16" s="2" t="inlineStr"/>
       <c r="D16" s="2" t="inlineStr"/>
       <c r="E16" s="2" t="inlineStr">
         <is>
-          <t>Poultry farms.</t>
+          <t>Poultry farms. Production mainly for eggs.</t>
         </is>
       </c>
       <c r="F16" s="2" t="inlineStr"/>
@@ -716,14 +712,14 @@
       <c r="A17" s="2" t="n"/>
       <c r="B17" s="2" t="inlineStr">
         <is>
-          <t>crustaceans</t>
+          <t>goats stud</t>
         </is>
       </c>
       <c r="C17" s="2" t="inlineStr"/>
       <c r="D17" s="2" t="inlineStr"/>
       <c r="E17" s="2" t="inlineStr">
         <is>
-          <t>Aquaculture: prawns, freshwater crayfish, etc.</t>
+          <t>Goats raised for sale as breeding animals.</t>
         </is>
       </c>
       <c r="F17" s="2" t="inlineStr"/>
@@ -732,14 +728,14 @@
       <c r="A18" s="2" t="n"/>
       <c r="B18" s="2" t="inlineStr">
         <is>
-          <t>turkeys</t>
+          <t>goats</t>
         </is>
       </c>
       <c r="C18" s="2" t="inlineStr"/>
       <c r="D18" s="2" t="inlineStr"/>
       <c r="E18" s="2" t="inlineStr">
         <is>
-          <t>Poultry farms.</t>
+          <t>Specify meat, dairy, stud, or wool where appropriate.</t>
         </is>
       </c>
       <c r="F18" s="2" t="inlineStr"/>
@@ -748,14 +744,14 @@
       <c r="A19" s="2" t="n"/>
       <c r="B19" s="2" t="inlineStr">
         <is>
-          <t>sheep dairy</t>
+          <t>goats wool</t>
         </is>
       </c>
       <c r="C19" s="2" t="inlineStr"/>
       <c r="D19" s="2" t="inlineStr"/>
       <c r="E19" s="2" t="inlineStr">
         <is>
-          <t>Sheep for milk production.</t>
+          <t>Goats for fibre production.</t>
         </is>
       </c>
       <c r="F19" s="2" t="inlineStr"/>
@@ -764,14 +760,14 @@
       <c r="A20" s="2" t="n"/>
       <c r="B20" s="2" t="inlineStr">
         <is>
-          <t>sheep stud</t>
+          <t>cats</t>
         </is>
       </c>
       <c r="C20" s="2" t="inlineStr"/>
       <c r="D20" s="2" t="inlineStr"/>
       <c r="E20" s="2" t="inlineStr">
         <is>
-          <t>Sheep raised for sale as breeding animals.</t>
+          <t>Includes cat breeding, catteries, or areas used for quarantine of cats related to import or export.</t>
         </is>
       </c>
       <c r="F20" s="2" t="inlineStr"/>
@@ -780,14 +776,14 @@
       <c r="A21" s="2" t="n"/>
       <c r="B21" s="2" t="inlineStr">
         <is>
-          <t>goats wool</t>
+          <t>pigs</t>
         </is>
       </c>
       <c r="C21" s="2" t="inlineStr"/>
       <c r="D21" s="2" t="inlineStr"/>
       <c r="E21" s="2" t="inlineStr">
         <is>
-          <t>Goats for fibre production.</t>
+          <t>Piggeries.</t>
         </is>
       </c>
       <c r="F21" s="2" t="inlineStr"/>
@@ -796,14 +792,14 @@
       <c r="A22" s="2" t="n"/>
       <c r="B22" s="2" t="inlineStr">
         <is>
-          <t>goats meat</t>
+          <t>sheep</t>
         </is>
       </c>
       <c r="C22" s="2" t="inlineStr"/>
       <c r="D22" s="2" t="inlineStr"/>
       <c r="E22" s="2" t="inlineStr">
         <is>
-          <t>Goats for meat production.</t>
+          <t>Specify meat, dairy, stud or wool where appropriate.</t>
         </is>
       </c>
       <c r="F22" s="2" t="inlineStr"/>
@@ -812,14 +808,14 @@
       <c r="A23" s="2" t="n"/>
       <c r="B23" s="2" t="inlineStr">
         <is>
-          <t>ducks</t>
+          <t>crocodiles</t>
         </is>
       </c>
       <c r="C23" s="2" t="inlineStr"/>
       <c r="D23" s="2" t="inlineStr"/>
       <c r="E23" s="2" t="inlineStr">
         <is>
-          <t>Poultry farms.</t>
+          <t>Aquaculture.</t>
         </is>
       </c>
       <c r="F23" s="2" t="inlineStr"/>
@@ -828,14 +824,14 @@
       <c r="A24" s="2" t="n"/>
       <c r="B24" s="2" t="inlineStr">
         <is>
-          <t>goats</t>
+          <t>horses</t>
         </is>
       </c>
       <c r="C24" s="2" t="inlineStr"/>
       <c r="D24" s="2" t="inlineStr"/>
       <c r="E24" s="2" t="inlineStr">
         <is>
-          <t>Specify meat, dairy, stud, or wool where appropriate.</t>
+          <t>Includes horse studs and recreational uses.</t>
         </is>
       </c>
       <c r="F24" s="2" t="inlineStr"/>
@@ -844,14 +840,14 @@
       <c r="A25" s="2" t="n"/>
       <c r="B25" s="2" t="inlineStr">
         <is>
-          <t>cattle meat</t>
+          <t>cattle stud</t>
         </is>
       </c>
       <c r="C25" s="2" t="inlineStr"/>
       <c r="D25" s="2" t="inlineStr"/>
       <c r="E25" s="2" t="inlineStr">
         <is>
-          <t>Cattle for meat (beef) production.</t>
+          <t>Cattle raised for sale as breeding animals.</t>
         </is>
       </c>
       <c r="F25" s="2" t="inlineStr"/>
@@ -876,14 +872,14 @@
       <c r="A27" s="2" t="n"/>
       <c r="B27" s="2" t="inlineStr">
         <is>
-          <t>cattle stud</t>
+          <t>dogs</t>
         </is>
       </c>
       <c r="C27" s="2" t="inlineStr"/>
       <c r="D27" s="2" t="inlineStr"/>
       <c r="E27" s="2" t="inlineStr">
         <is>
-          <t>Cattle raised for sale as breeding animals.</t>
+          <t>Includes dog breeding, kennels, or areas used for quarantine of dogs related to import or export.</t>
         </is>
       </c>
       <c r="F27" s="2" t="inlineStr"/>
@@ -908,14 +904,14 @@
       <c r="A29" s="2" t="n"/>
       <c r="B29" s="2" t="inlineStr">
         <is>
-          <t>horses</t>
+          <t>goats dairy</t>
         </is>
       </c>
       <c r="C29" s="2" t="inlineStr"/>
       <c r="D29" s="2" t="inlineStr"/>
       <c r="E29" s="2" t="inlineStr">
         <is>
-          <t>Includes horse studs and recreational uses.</t>
+          <t>Goats for milk production.</t>
         </is>
       </c>
       <c r="F29" s="2" t="inlineStr"/>
@@ -924,26 +920,30 @@
       <c r="A30" s="2" t="n"/>
       <c r="B30" s="2" t="inlineStr">
         <is>
-          <t>deer</t>
+          <t>geese</t>
         </is>
       </c>
       <c r="C30" s="2" t="inlineStr"/>
       <c r="D30" s="2" t="inlineStr"/>
-      <c r="E30" s="2" t="inlineStr"/>
+      <c r="E30" s="2" t="inlineStr">
+        <is>
+          <t>Poultry farms.</t>
+        </is>
+      </c>
       <c r="F30" s="2" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n"/>
       <c r="B31" s="2" t="inlineStr">
         <is>
-          <t>chickens eggs</t>
+          <t>chickens</t>
         </is>
       </c>
       <c r="C31" s="2" t="inlineStr"/>
       <c r="D31" s="2" t="inlineStr"/>
       <c r="E31" s="2" t="inlineStr">
         <is>
-          <t>Poultry farms. Production mainly for eggs.</t>
+          <t>Poultry farms. Specify whether for eggs or meat where possible.</t>
         </is>
       </c>
       <c r="F31" s="2" t="inlineStr"/>
@@ -952,14 +952,14 @@
       <c r="A32" s="2" t="n"/>
       <c r="B32" s="2" t="inlineStr">
         <is>
-          <t>sheep wool</t>
+          <t>ducks</t>
         </is>
       </c>
       <c r="C32" s="2" t="inlineStr"/>
       <c r="D32" s="2" t="inlineStr"/>
       <c r="E32" s="2" t="inlineStr">
         <is>
-          <t>Sheep for fibre production.</t>
+          <t>Poultry farms.</t>
         </is>
       </c>
       <c r="F32" s="2" t="inlineStr"/>
@@ -968,14 +968,14 @@
       <c r="A33" s="2" t="n"/>
       <c r="B33" s="2" t="inlineStr">
         <is>
-          <t>goats stud</t>
+          <t>goats meat</t>
         </is>
       </c>
       <c r="C33" s="2" t="inlineStr"/>
       <c r="D33" s="2" t="inlineStr"/>
       <c r="E33" s="2" t="inlineStr">
         <is>
-          <t>Goats raised for sale as breeding animals.</t>
+          <t>Goats for meat production.</t>
         </is>
       </c>
       <c r="F33" s="2" t="inlineStr"/>
@@ -988,19 +988,23 @@
       </c>
       <c r="B34" s="2" t="inlineStr">
         <is>
-          <t>barley</t>
+          <t>buckwheat</t>
         </is>
       </c>
       <c r="C34" s="2" t="inlineStr"/>
       <c r="D34" s="2" t="inlineStr"/>
-      <c r="E34" s="2" t="inlineStr"/>
+      <c r="E34" s="2" t="inlineStr">
+        <is>
+          <t>Buckwheat is a pseudocereal related to rhubarb. As it is grown as a grain it is considered part of cereals.</t>
+        </is>
+      </c>
       <c r="F34" s="2" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n"/>
       <c r="B35" s="2" t="inlineStr">
         <is>
-          <t>canary_seed</t>
+          <t>rice</t>
         </is>
       </c>
       <c r="C35" s="2" t="inlineStr"/>
@@ -1012,7 +1016,7 @@
       <c r="A36" s="2" t="n"/>
       <c r="B36" s="2" t="inlineStr">
         <is>
-          <t>rye cereal</t>
+          <t>triticale</t>
         </is>
       </c>
       <c r="C36" s="2" t="inlineStr"/>
@@ -1036,7 +1040,7 @@
       <c r="A38" s="2" t="n"/>
       <c r="B38" s="2" t="inlineStr">
         <is>
-          <t>triticale</t>
+          <t>millet and pancium</t>
         </is>
       </c>
       <c r="C38" s="2" t="inlineStr"/>
@@ -1048,30 +1052,26 @@
       <c r="A39" s="2" t="n"/>
       <c r="B39" s="2" t="inlineStr">
         <is>
-          <t>sorghum grain</t>
+          <t>barley</t>
         </is>
       </c>
       <c r="C39" s="2" t="inlineStr"/>
       <c r="D39" s="2" t="inlineStr"/>
-      <c r="E39" s="2" t="inlineStr">
-        <is>
-          <t>Sorghum grown for grain. Excludes forage sorghum.</t>
-        </is>
-      </c>
+      <c r="E39" s="2" t="inlineStr"/>
       <c r="F39" s="2" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n"/>
       <c r="B40" s="2" t="inlineStr">
         <is>
-          <t>buckwheat</t>
+          <t>quinoa</t>
         </is>
       </c>
       <c r="C40" s="2" t="inlineStr"/>
       <c r="D40" s="2" t="inlineStr"/>
       <c r="E40" s="2" t="inlineStr">
         <is>
-          <t>Buckwheat is a pseudocereal related to rhubarb. As it is grown as a grain it is considered part of cereals.</t>
+          <t>Quinoa is a pseudocereal related to beetroot, spinach and tumbleweeds. As it is grown as a grain it is considered part of cereals.</t>
         </is>
       </c>
       <c r="F40" s="2" t="inlineStr"/>
@@ -1080,14 +1080,14 @@
       <c r="A41" s="2" t="n"/>
       <c r="B41" s="2" t="inlineStr">
         <is>
-          <t>quinoa</t>
+          <t>sorghum grain</t>
         </is>
       </c>
       <c r="C41" s="2" t="inlineStr"/>
       <c r="D41" s="2" t="inlineStr"/>
       <c r="E41" s="2" t="inlineStr">
         <is>
-          <t>Quinoa is a pseudocereal related to beetroot, spinach and tumbleweeds. As it is grown as a grain it is considered part of cereals.</t>
+          <t>Sorghum grown for grain. Excludes forage sorghum.</t>
         </is>
       </c>
       <c r="F41" s="2" t="inlineStr"/>
@@ -1096,7 +1096,7 @@
       <c r="A42" s="2" t="n"/>
       <c r="B42" s="2" t="inlineStr">
         <is>
-          <t>millet and pancium</t>
+          <t>wheat</t>
         </is>
       </c>
       <c r="C42" s="2" t="inlineStr"/>
@@ -1108,7 +1108,7 @@
       <c r="A43" s="2" t="n"/>
       <c r="B43" s="2" t="inlineStr">
         <is>
-          <t>wheat</t>
+          <t>maize</t>
         </is>
       </c>
       <c r="C43" s="2" t="inlineStr"/>
@@ -1120,7 +1120,7 @@
       <c r="A44" s="2" t="n"/>
       <c r="B44" s="2" t="inlineStr">
         <is>
-          <t>maize</t>
+          <t>canary_seed</t>
         </is>
       </c>
       <c r="C44" s="2" t="inlineStr"/>
@@ -1132,7 +1132,7 @@
       <c r="A45" s="2" t="n"/>
       <c r="B45" s="2" t="inlineStr">
         <is>
-          <t>rice</t>
+          <t>rye cereal</t>
         </is>
       </c>
       <c r="C45" s="2" t="inlineStr"/>
@@ -1148,7 +1148,7 @@
       </c>
       <c r="B46" s="2" t="inlineStr">
         <is>
-          <t>coffee</t>
+          <t>essential oil crops</t>
         </is>
       </c>
       <c r="C46" s="2" t="inlineStr"/>
@@ -1160,7 +1160,7 @@
       <c r="A47" s="2" t="n"/>
       <c r="B47" s="2" t="inlineStr">
         <is>
-          <t>oil palms</t>
+          <t>tea</t>
         </is>
       </c>
       <c r="C47" s="2" t="inlineStr"/>
@@ -1184,7 +1184,7 @@
       <c r="A49" s="2" t="n"/>
       <c r="B49" s="2" t="inlineStr">
         <is>
-          <t>horseradish</t>
+          <t>cocoa</t>
         </is>
       </c>
       <c r="C49" s="2" t="inlineStr"/>
@@ -1196,7 +1196,7 @@
       <c r="A50" s="2" t="n"/>
       <c r="B50" s="2" t="inlineStr">
         <is>
-          <t>pyrethrum</t>
+          <t>wasabi</t>
         </is>
       </c>
       <c r="C50" s="2" t="inlineStr"/>
@@ -1220,7 +1220,7 @@
       <c r="A52" s="2" t="n"/>
       <c r="B52" s="2" t="inlineStr">
         <is>
-          <t>wasabi</t>
+          <t>hops</t>
         </is>
       </c>
       <c r="C52" s="2" t="inlineStr"/>
@@ -1232,7 +1232,7 @@
       <c r="A53" s="2" t="n"/>
       <c r="B53" s="2" t="inlineStr">
         <is>
-          <t>tobacco</t>
+          <t>sugar cane</t>
         </is>
       </c>
       <c r="C53" s="2" t="inlineStr"/>
@@ -1244,7 +1244,7 @@
       <c r="A54" s="2" t="n"/>
       <c r="B54" s="2" t="inlineStr">
         <is>
-          <t>ginger</t>
+          <t>coffee</t>
         </is>
       </c>
       <c r="C54" s="2" t="inlineStr"/>
@@ -1256,7 +1256,7 @@
       <c r="A55" s="2" t="n"/>
       <c r="B55" s="2" t="inlineStr">
         <is>
-          <t>pepper</t>
+          <t xml:space="preserve">poppies </t>
         </is>
       </c>
       <c r="C55" s="2" t="inlineStr"/>
@@ -1268,7 +1268,7 @@
       <c r="A56" s="2" t="n"/>
       <c r="B56" s="2" t="inlineStr">
         <is>
-          <t>cotton</t>
+          <t>tobacco</t>
         </is>
       </c>
       <c r="C56" s="2" t="inlineStr"/>
@@ -1280,7 +1280,7 @@
       <c r="A57" s="2" t="n"/>
       <c r="B57" s="2" t="inlineStr">
         <is>
-          <t>cotton seed</t>
+          <t>horseradish</t>
         </is>
       </c>
       <c r="C57" s="2" t="inlineStr"/>
@@ -1292,7 +1292,7 @@
       <c r="A58" s="2" t="n"/>
       <c r="B58" s="2" t="inlineStr">
         <is>
-          <t>cocoa</t>
+          <t>cotton seed</t>
         </is>
       </c>
       <c r="C58" s="2" t="inlineStr"/>
@@ -1304,7 +1304,7 @@
       <c r="A59" s="2" t="n"/>
       <c r="B59" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">poppies </t>
+          <t>pyrethrum</t>
         </is>
       </c>
       <c r="C59" s="2" t="inlineStr"/>
@@ -1316,7 +1316,7 @@
       <c r="A60" s="2" t="n"/>
       <c r="B60" s="2" t="inlineStr">
         <is>
-          <t>sugar cane</t>
+          <t>ginger</t>
         </is>
       </c>
       <c r="C60" s="2" t="inlineStr"/>
@@ -1328,7 +1328,7 @@
       <c r="A61" s="2" t="n"/>
       <c r="B61" s="2" t="inlineStr">
         <is>
-          <t>essential oil crops</t>
+          <t>pharmaceutical and cosmetic plants</t>
         </is>
       </c>
       <c r="C61" s="2" t="inlineStr"/>
@@ -1340,7 +1340,7 @@
       <c r="A62" s="2" t="n"/>
       <c r="B62" s="2" t="inlineStr">
         <is>
-          <t>tea</t>
+          <t>oil palms</t>
         </is>
       </c>
       <c r="C62" s="2" t="inlineStr"/>
@@ -1352,7 +1352,7 @@
       <c r="A63" s="2" t="n"/>
       <c r="B63" s="2" t="inlineStr">
         <is>
-          <t>hops</t>
+          <t>pepper</t>
         </is>
       </c>
       <c r="C63" s="2" t="inlineStr"/>
@@ -1364,7 +1364,7 @@
       <c r="A64" s="2" t="n"/>
       <c r="B64" s="2" t="inlineStr">
         <is>
-          <t>pharmaceutical and cosmetic plants</t>
+          <t>cotton</t>
         </is>
       </c>
       <c r="C64" s="2" t="inlineStr"/>
@@ -1392,7 +1392,7 @@
       <c r="A66" s="2" t="n"/>
       <c r="B66" s="2" t="inlineStr">
         <is>
-          <t>flowers and foliage</t>
+          <t>proteas</t>
         </is>
       </c>
       <c r="C66" s="2" t="inlineStr"/>
@@ -1404,7 +1404,7 @@
       <c r="A67" s="2" t="n"/>
       <c r="B67" s="2" t="inlineStr">
         <is>
-          <t>orchids</t>
+          <t>carnations</t>
         </is>
       </c>
       <c r="C67" s="2" t="inlineStr"/>
@@ -1416,7 +1416,7 @@
       <c r="A68" s="2" t="n"/>
       <c r="B68" s="2" t="inlineStr">
         <is>
-          <t>calendula</t>
+          <t>lavender</t>
         </is>
       </c>
       <c r="C68" s="2" t="inlineStr"/>
@@ -1428,7 +1428,7 @@
       <c r="A69" s="2" t="n"/>
       <c r="B69" s="2" t="inlineStr">
         <is>
-          <t>proteas</t>
+          <t>lilies</t>
         </is>
       </c>
       <c r="C69" s="2" t="inlineStr"/>
@@ -1440,7 +1440,7 @@
       <c r="A70" s="2" t="n"/>
       <c r="B70" s="2" t="inlineStr">
         <is>
-          <t>chrysanthemums</t>
+          <t>roses</t>
         </is>
       </c>
       <c r="C70" s="2" t="inlineStr"/>
@@ -1452,7 +1452,7 @@
       <c r="A71" s="2" t="n"/>
       <c r="B71" s="2" t="inlineStr">
         <is>
-          <t>australian native flowers</t>
+          <t>tropical flowers</t>
         </is>
       </c>
       <c r="C71" s="2" t="inlineStr"/>
@@ -1464,7 +1464,7 @@
       <c r="A72" s="2" t="n"/>
       <c r="B72" s="2" t="inlineStr">
         <is>
-          <t>gerberas</t>
+          <t>chrysanthemums</t>
         </is>
       </c>
       <c r="C72" s="2" t="inlineStr"/>
@@ -1476,7 +1476,7 @@
       <c r="A73" s="2" t="n"/>
       <c r="B73" s="2" t="inlineStr">
         <is>
-          <t>tulips</t>
+          <t>calendula</t>
         </is>
       </c>
       <c r="C73" s="2" t="inlineStr"/>
@@ -1488,7 +1488,7 @@
       <c r="A74" s="2" t="n"/>
       <c r="B74" s="2" t="inlineStr">
         <is>
-          <t>lavender</t>
+          <t>tulips</t>
         </is>
       </c>
       <c r="C74" s="2" t="inlineStr"/>
@@ -1500,7 +1500,7 @@
       <c r="A75" s="2" t="n"/>
       <c r="B75" s="2" t="inlineStr">
         <is>
-          <t>roses</t>
+          <t>daffodils</t>
         </is>
       </c>
       <c r="C75" s="2" t="inlineStr"/>
@@ -1512,7 +1512,7 @@
       <c r="A76" s="2" t="n"/>
       <c r="B76" s="2" t="inlineStr">
         <is>
-          <t>tropical flowers</t>
+          <t>gerberas</t>
         </is>
       </c>
       <c r="C76" s="2" t="inlineStr"/>
@@ -1524,7 +1524,7 @@
       <c r="A77" s="2" t="n"/>
       <c r="B77" s="2" t="inlineStr">
         <is>
-          <t>carnations</t>
+          <t>australian native flowers</t>
         </is>
       </c>
       <c r="C77" s="2" t="inlineStr"/>
@@ -1536,7 +1536,7 @@
       <c r="A78" s="2" t="n"/>
       <c r="B78" s="2" t="inlineStr">
         <is>
-          <t>lilies</t>
+          <t>flowers and foliage</t>
         </is>
       </c>
       <c r="C78" s="2" t="inlineStr"/>
@@ -1548,7 +1548,7 @@
       <c r="A79" s="2" t="n"/>
       <c r="B79" s="2" t="inlineStr">
         <is>
-          <t>daffodils</t>
+          <t>orchids</t>
         </is>
       </c>
       <c r="C79" s="2" t="inlineStr"/>
@@ -1564,15 +1564,11 @@
       </c>
       <c r="B80" s="2" t="inlineStr">
         <is>
-          <t>carbon forest standard</t>
+          <t>christmas trees</t>
         </is>
       </c>
       <c r="C80" s="2" t="inlineStr"/>
-      <c r="D80" s="2" t="inlineStr">
-        <is>
-          <t>Standard carbon foresty under the ETS. Standard forestry refers to post-1989 forests under the ETS that are expected to be regularly harvested and replanted, such as commercial plantation forests. Other commodities (such as sawlog) are compatible.</t>
-        </is>
-      </c>
+      <c r="D80" s="2" t="inlineStr"/>
       <c r="E80" s="2" t="inlineStr"/>
       <c r="F80" s="2" t="inlineStr"/>
     </row>
@@ -1580,7 +1576,7 @@
       <c r="A81" s="2" t="n"/>
       <c r="B81" s="2" t="inlineStr">
         <is>
-          <t>bamboo</t>
+          <t>sandalwood</t>
         </is>
       </c>
       <c r="C81" s="2" t="inlineStr"/>
@@ -1592,15 +1588,11 @@
       <c r="A82" s="2" t="n"/>
       <c r="B82" s="2" t="inlineStr">
         <is>
-          <t>carbon forest permanent</t>
+          <t>bamboo</t>
         </is>
       </c>
       <c r="C82" s="2" t="inlineStr"/>
-      <c r="D82" s="2" t="inlineStr">
-        <is>
-          <t>Permanent carbon forestry under the ETS. These are post-1989 forests that will not be clear-felled. They are expected to remain in permanent forestry for at least 50 years. Before 1 January 2023, the ETS didn't distinguish between standard and permanent forestry. Post-1989 forest land that entered the ETS before 1 January 2023 is standard forestry, unless an application has been accepted to change it to permanent forestry.</t>
-        </is>
-      </c>
+      <c r="D82" s="2" t="inlineStr"/>
       <c r="E82" s="2" t="inlineStr"/>
       <c r="F82" s="2" t="inlineStr"/>
     </row>
@@ -1608,7 +1600,7 @@
       <c r="A83" s="2" t="n"/>
       <c r="B83" s="2" t="inlineStr">
         <is>
-          <t>tea tree</t>
+          <t>eucalyptus oil</t>
         </is>
       </c>
       <c r="C83" s="2" t="inlineStr"/>
@@ -1620,7 +1612,7 @@
       <c r="A84" s="2" t="n"/>
       <c r="B84" s="2" t="inlineStr">
         <is>
-          <t>sandalwood</t>
+          <t>tea tree</t>
         </is>
       </c>
       <c r="C84" s="2" t="inlineStr"/>
@@ -1632,7 +1624,7 @@
       <c r="A85" s="2" t="n"/>
       <c r="B85" s="2" t="inlineStr">
         <is>
-          <t>sawlogs</t>
+          <t>oil mallee</t>
         </is>
       </c>
       <c r="C85" s="2" t="inlineStr"/>
@@ -1644,7 +1636,7 @@
       <c r="A86" s="2" t="n"/>
       <c r="B86" s="2" t="inlineStr">
         <is>
-          <t>christmas trees</t>
+          <t>pulp wood</t>
         </is>
       </c>
       <c r="C86" s="2" t="inlineStr"/>
@@ -1656,7 +1648,7 @@
       <c r="A87" s="2" t="n"/>
       <c r="B87" s="2" t="inlineStr">
         <is>
-          <t>eucalyptus oil</t>
+          <t>sawlogs</t>
         </is>
       </c>
       <c r="C87" s="2" t="inlineStr"/>
@@ -1668,11 +1660,15 @@
       <c r="A88" s="2" t="n"/>
       <c r="B88" s="2" t="inlineStr">
         <is>
-          <t>oil mallee</t>
+          <t>carbon forest permanent</t>
         </is>
       </c>
       <c r="C88" s="2" t="inlineStr"/>
-      <c r="D88" s="2" t="inlineStr"/>
+      <c r="D88" s="2" t="inlineStr">
+        <is>
+          <t>Permanent carbon forestry under the ETS. These are post-1989 forests that will not be clear-felled. They are expected to remain in permanent forestry for at least 50 years. Before 1 January 2023, the ETS didn't distinguish between standard and permanent forestry. Post-1989 forest land that entered the ETS before 1 January 2023 is standard forestry, unless an application has been accepted to change it to permanent forestry.</t>
+        </is>
+      </c>
       <c r="E88" s="2" t="inlineStr"/>
       <c r="F88" s="2" t="inlineStr"/>
     </row>
@@ -1680,11 +1676,15 @@
       <c r="A89" s="2" t="n"/>
       <c r="B89" s="2" t="inlineStr">
         <is>
-          <t>pulp wood</t>
+          <t>carbon forest standard</t>
         </is>
       </c>
       <c r="C89" s="2" t="inlineStr"/>
-      <c r="D89" s="2" t="inlineStr"/>
+      <c r="D89" s="2" t="inlineStr">
+        <is>
+          <t>Standard carbon foresty under the ETS. Standard forestry refers to post-1989 forests under the ETS that are expected to be regularly harvested and replanted, such as commercial plantation forests. Other commodities (such as sawlog) are compatible.</t>
+        </is>
+      </c>
       <c r="E89" s="2" t="inlineStr"/>
       <c r="F89" s="2" t="inlineStr"/>
     </row>
@@ -1696,7 +1696,7 @@
       </c>
       <c r="B90" s="2" t="inlineStr">
         <is>
-          <t>mulberries</t>
+          <t>cranberries</t>
         </is>
       </c>
       <c r="C90" s="2" t="inlineStr"/>
@@ -1708,7 +1708,7 @@
       <c r="A91" s="2" t="n"/>
       <c r="B91" s="2" t="inlineStr">
         <is>
-          <t>boysenberries</t>
+          <t>pineapples</t>
         </is>
       </c>
       <c r="C91" s="2" t="inlineStr"/>
@@ -1720,7 +1720,7 @@
       <c r="A92" s="2" t="n"/>
       <c r="B92" s="2" t="inlineStr">
         <is>
-          <t>custard apples</t>
+          <t>persimmons</t>
         </is>
       </c>
       <c r="C92" s="2" t="inlineStr"/>
@@ -1732,7 +1732,7 @@
       <c r="A93" s="2" t="n"/>
       <c r="B93" s="2" t="inlineStr">
         <is>
-          <t>jackfruit</t>
+          <t>blackcurrants</t>
         </is>
       </c>
       <c r="C93" s="2" t="inlineStr"/>
@@ -1744,7 +1744,7 @@
       <c r="A94" s="2" t="n"/>
       <c r="B94" s="2" t="inlineStr">
         <is>
-          <t>oranges</t>
+          <t>babacos</t>
         </is>
       </c>
       <c r="C94" s="2" t="inlineStr"/>
@@ -1756,7 +1756,7 @@
       <c r="A95" s="2" t="n"/>
       <c r="B95" s="2" t="inlineStr">
         <is>
-          <t>pawpaws</t>
+          <t>loquats</t>
         </is>
       </c>
       <c r="C95" s="2" t="inlineStr"/>
@@ -1768,7 +1768,7 @@
       <c r="A96" s="2" t="n"/>
       <c r="B96" s="2" t="inlineStr">
         <is>
-          <t>dragon fruit</t>
+          <t>boysenberries</t>
         </is>
       </c>
       <c r="C96" s="2" t="inlineStr"/>
@@ -1780,7 +1780,7 @@
       <c r="A97" s="2" t="n"/>
       <c r="B97" s="2" t="inlineStr">
         <is>
-          <t>lemons</t>
+          <t>mulberries</t>
         </is>
       </c>
       <c r="C97" s="2" t="inlineStr"/>
@@ -1792,7 +1792,7 @@
       <c r="A98" s="2" t="n"/>
       <c r="B98" s="2" t="inlineStr">
         <is>
-          <t>pears</t>
+          <t>apples</t>
         </is>
       </c>
       <c r="C98" s="2" t="inlineStr"/>
@@ -1804,7 +1804,7 @@
       <c r="A99" s="2" t="n"/>
       <c r="B99" s="2" t="inlineStr">
         <is>
-          <t>kiwifruit</t>
+          <t>mangosteen</t>
         </is>
       </c>
       <c r="C99" s="2" t="inlineStr"/>
@@ -1816,7 +1816,7 @@
       <c r="A100" s="2" t="n"/>
       <c r="B100" s="2" t="inlineStr">
         <is>
-          <t>pepinos</t>
+          <t>peacharines</t>
         </is>
       </c>
       <c r="C100" s="2" t="inlineStr"/>
@@ -1828,7 +1828,7 @@
       <c r="A101" s="2" t="n"/>
       <c r="B101" s="2" t="inlineStr">
         <is>
-          <t>apricots</t>
+          <t>coconut</t>
         </is>
       </c>
       <c r="C101" s="2" t="inlineStr"/>
@@ -1840,7 +1840,7 @@
       <c r="A102" s="2" t="n"/>
       <c r="B102" s="2" t="inlineStr">
         <is>
-          <t>pineapples</t>
+          <t>chokos</t>
         </is>
       </c>
       <c r="C102" s="2" t="inlineStr"/>
@@ -1852,7 +1852,7 @@
       <c r="A103" s="2" t="n"/>
       <c r="B103" s="2" t="inlineStr">
         <is>
-          <t>persimmons</t>
+          <t>lychees</t>
         </is>
       </c>
       <c r="C103" s="2" t="inlineStr"/>
@@ -1864,7 +1864,7 @@
       <c r="A104" s="2" t="n"/>
       <c r="B104" s="2" t="inlineStr">
         <is>
-          <t>watermelons</t>
+          <t>grapes</t>
         </is>
       </c>
       <c r="C104" s="2" t="inlineStr"/>
@@ -1876,7 +1876,7 @@
       <c r="A105" s="2" t="n"/>
       <c r="B105" s="2" t="inlineStr">
         <is>
-          <t>longans</t>
+          <t>apricots</t>
         </is>
       </c>
       <c r="C105" s="2" t="inlineStr"/>
@@ -1888,7 +1888,7 @@
       <c r="A106" s="2" t="n"/>
       <c r="B106" s="2" t="inlineStr">
         <is>
-          <t>feijoa</t>
+          <t>mangoes</t>
         </is>
       </c>
       <c r="C106" s="2" t="inlineStr"/>
@@ -1900,7 +1900,7 @@
       <c r="A107" s="2" t="n"/>
       <c r="B107" s="2" t="inlineStr">
         <is>
-          <t>guavas</t>
+          <t>olives</t>
         </is>
       </c>
       <c r="C107" s="2" t="inlineStr"/>
@@ -1912,7 +1912,7 @@
       <c r="A108" s="2" t="n"/>
       <c r="B108" s="2" t="inlineStr">
         <is>
-          <t>lychees</t>
+          <t>plums</t>
         </is>
       </c>
       <c r="C108" s="2" t="inlineStr"/>
@@ -1924,7 +1924,7 @@
       <c r="A109" s="2" t="n"/>
       <c r="B109" s="2" t="inlineStr">
         <is>
-          <t>mangoes</t>
+          <t>guavas</t>
         </is>
       </c>
       <c r="C109" s="2" t="inlineStr"/>
@@ -1936,7 +1936,7 @@
       <c r="A110" s="2" t="n"/>
       <c r="B110" s="2" t="inlineStr">
         <is>
-          <t>chokos</t>
+          <t>grapes wine</t>
         </is>
       </c>
       <c r="C110" s="2" t="inlineStr"/>
@@ -1948,7 +1948,7 @@
       <c r="A111" s="2" t="n"/>
       <c r="B111" s="2" t="inlineStr">
         <is>
-          <t>blackcurrants</t>
+          <t>oranges</t>
         </is>
       </c>
       <c r="C111" s="2" t="inlineStr"/>
@@ -1960,7 +1960,7 @@
       <c r="A112" s="2" t="n"/>
       <c r="B112" s="2" t="inlineStr">
         <is>
-          <t>melons</t>
+          <t>pawpaws</t>
         </is>
       </c>
       <c r="C112" s="2" t="inlineStr"/>
@@ -1972,7 +1972,7 @@
       <c r="A113" s="2" t="n"/>
       <c r="B113" s="2" t="inlineStr">
         <is>
-          <t>coconut</t>
+          <t>quinces</t>
         </is>
       </c>
       <c r="C113" s="2" t="inlineStr"/>
@@ -1984,7 +1984,7 @@
       <c r="A114" s="2" t="n"/>
       <c r="B114" s="2" t="inlineStr">
         <is>
-          <t>passionfruit</t>
+          <t>mandarins</t>
         </is>
       </c>
       <c r="C114" s="2" t="inlineStr"/>
@@ -1996,7 +1996,7 @@
       <c r="A115" s="2" t="n"/>
       <c r="B115" s="2" t="inlineStr">
         <is>
-          <t>pomegranate</t>
+          <t>redcurrants</t>
         </is>
       </c>
       <c r="C115" s="2" t="inlineStr"/>
@@ -2008,7 +2008,7 @@
       <c r="A116" s="2" t="n"/>
       <c r="B116" s="2" t="inlineStr">
         <is>
-          <t>pears nashi</t>
+          <t>tangelos</t>
         </is>
       </c>
       <c r="C116" s="2" t="inlineStr"/>
@@ -2020,7 +2020,7 @@
       <c r="A117" s="2" t="n"/>
       <c r="B117" s="2" t="inlineStr">
         <is>
-          <t>blueberries</t>
+          <t>grapes table</t>
         </is>
       </c>
       <c r="C117" s="2" t="inlineStr"/>
@@ -2032,7 +2032,7 @@
       <c r="A118" s="2" t="n"/>
       <c r="B118" s="2" t="inlineStr">
         <is>
-          <t>tangelos</t>
+          <t>pomegranate</t>
         </is>
       </c>
       <c r="C118" s="2" t="inlineStr"/>
@@ -2044,7 +2044,7 @@
       <c r="A119" s="2" t="n"/>
       <c r="B119" s="2" t="inlineStr">
         <is>
-          <t>gooseberries</t>
+          <t>passionfruit</t>
         </is>
       </c>
       <c r="C119" s="2" t="inlineStr"/>
@@ -2056,7 +2056,7 @@
       <c r="A120" s="2" t="n"/>
       <c r="B120" s="2" t="inlineStr">
         <is>
-          <t>carambolas</t>
+          <t>kiwifruit</t>
         </is>
       </c>
       <c r="C120" s="2" t="inlineStr"/>
@@ -2068,7 +2068,7 @@
       <c r="A121" s="2" t="n"/>
       <c r="B121" s="2" t="inlineStr">
         <is>
-          <t>cranberries</t>
+          <t>gooseberries</t>
         </is>
       </c>
       <c r="C121" s="2" t="inlineStr"/>
@@ -2080,7 +2080,7 @@
       <c r="A122" s="2" t="n"/>
       <c r="B122" s="2" t="inlineStr">
         <is>
-          <t>grapefruit</t>
+          <t>peaches</t>
         </is>
       </c>
       <c r="C122" s="2" t="inlineStr"/>
@@ -2092,7 +2092,7 @@
       <c r="A123" s="2" t="n"/>
       <c r="B123" s="2" t="inlineStr">
         <is>
-          <t>peacharines</t>
+          <t>feijoa</t>
         </is>
       </c>
       <c r="C123" s="2" t="inlineStr"/>
@@ -2104,7 +2104,7 @@
       <c r="A124" s="2" t="n"/>
       <c r="B124" s="2" t="inlineStr">
         <is>
-          <t>raspberries</t>
+          <t>kumquat</t>
         </is>
       </c>
       <c r="C124" s="2" t="inlineStr"/>
@@ -2116,7 +2116,7 @@
       <c r="A125" s="2" t="n"/>
       <c r="B125" s="2" t="inlineStr">
         <is>
-          <t>loquats</t>
+          <t>limes</t>
         </is>
       </c>
       <c r="C125" s="2" t="inlineStr"/>
@@ -2128,7 +2128,7 @@
       <c r="A126" s="2" t="n"/>
       <c r="B126" s="2" t="inlineStr">
         <is>
-          <t>olives</t>
+          <t>nectarines</t>
         </is>
       </c>
       <c r="C126" s="2" t="inlineStr"/>
@@ -2152,7 +2152,7 @@
       <c r="A128" s="2" t="n"/>
       <c r="B128" s="2" t="inlineStr">
         <is>
-          <t>rosella</t>
+          <t>bananas</t>
         </is>
       </c>
       <c r="C128" s="2" t="inlineStr"/>
@@ -2164,7 +2164,7 @@
       <c r="A129" s="2" t="n"/>
       <c r="B129" s="2" t="inlineStr">
         <is>
-          <t>babacos</t>
+          <t>custard apples</t>
         </is>
       </c>
       <c r="C129" s="2" t="inlineStr"/>
@@ -2176,7 +2176,7 @@
       <c r="A130" s="2" t="n"/>
       <c r="B130" s="2" t="inlineStr">
         <is>
-          <t>figs</t>
+          <t>cherries</t>
         </is>
       </c>
       <c r="C130" s="2" t="inlineStr"/>
@@ -2188,7 +2188,7 @@
       <c r="A131" s="2" t="n"/>
       <c r="B131" s="2" t="inlineStr">
         <is>
-          <t>grapes</t>
+          <t>loganberries</t>
         </is>
       </c>
       <c r="C131" s="2" t="inlineStr"/>
@@ -2200,7 +2200,7 @@
       <c r="A132" s="2" t="n"/>
       <c r="B132" s="2" t="inlineStr">
         <is>
-          <t>apples</t>
+          <t>pears nashi</t>
         </is>
       </c>
       <c r="C132" s="2" t="inlineStr"/>
@@ -2212,7 +2212,7 @@
       <c r="A133" s="2" t="n"/>
       <c r="B133" s="2" t="inlineStr">
         <is>
-          <t>strawberries</t>
+          <t>pears</t>
         </is>
       </c>
       <c r="C133" s="2" t="inlineStr"/>
@@ -2224,7 +2224,7 @@
       <c r="A134" s="2" t="n"/>
       <c r="B134" s="2" t="inlineStr">
         <is>
-          <t>blackberries</t>
+          <t>rosella</t>
         </is>
       </c>
       <c r="C134" s="2" t="inlineStr"/>
@@ -2236,7 +2236,7 @@
       <c r="A135" s="2" t="n"/>
       <c r="B135" s="2" t="inlineStr">
         <is>
-          <t>kumquat</t>
+          <t>carambolas</t>
         </is>
       </c>
       <c r="C135" s="2" t="inlineStr"/>
@@ -2248,7 +2248,7 @@
       <c r="A136" s="2" t="n"/>
       <c r="B136" s="2" t="inlineStr">
         <is>
-          <t>peaches</t>
+          <t>lemons</t>
         </is>
       </c>
       <c r="C136" s="2" t="inlineStr"/>
@@ -2260,7 +2260,7 @@
       <c r="A137" s="2" t="n"/>
       <c r="B137" s="2" t="inlineStr">
         <is>
-          <t>dates</t>
+          <t>melons</t>
         </is>
       </c>
       <c r="C137" s="2" t="inlineStr"/>
@@ -2272,7 +2272,7 @@
       <c r="A138" s="2" t="n"/>
       <c r="B138" s="2" t="inlineStr">
         <is>
-          <t>nectarines</t>
+          <t>dates</t>
         </is>
       </c>
       <c r="C138" s="2" t="inlineStr"/>
@@ -2284,7 +2284,7 @@
       <c r="A139" s="2" t="n"/>
       <c r="B139" s="2" t="inlineStr">
         <is>
-          <t>cherries</t>
+          <t>pepinos</t>
         </is>
       </c>
       <c r="C139" s="2" t="inlineStr"/>
@@ -2296,7 +2296,7 @@
       <c r="A140" s="2" t="n"/>
       <c r="B140" s="2" t="inlineStr">
         <is>
-          <t>limes</t>
+          <t>watermelons</t>
         </is>
       </c>
       <c r="C140" s="2" t="inlineStr"/>
@@ -2308,7 +2308,7 @@
       <c r="A141" s="2" t="n"/>
       <c r="B141" s="2" t="inlineStr">
         <is>
-          <t>redcurrants</t>
+          <t>jackfruit</t>
         </is>
       </c>
       <c r="C141" s="2" t="inlineStr"/>
@@ -2320,7 +2320,7 @@
       <c r="A142" s="2" t="n"/>
       <c r="B142" s="2" t="inlineStr">
         <is>
-          <t>mangosteen</t>
+          <t>blackberries</t>
         </is>
       </c>
       <c r="C142" s="2" t="inlineStr"/>
@@ -2332,7 +2332,7 @@
       <c r="A143" s="2" t="n"/>
       <c r="B143" s="2" t="inlineStr">
         <is>
-          <t>grapes dried</t>
+          <t>longans</t>
         </is>
       </c>
       <c r="C143" s="2" t="inlineStr"/>
@@ -2344,7 +2344,7 @@
       <c r="A144" s="2" t="n"/>
       <c r="B144" s="2" t="inlineStr">
         <is>
-          <t>quinces</t>
+          <t>raspberries</t>
         </is>
       </c>
       <c r="C144" s="2" t="inlineStr"/>
@@ -2356,7 +2356,7 @@
       <c r="A145" s="2" t="n"/>
       <c r="B145" s="2" t="inlineStr">
         <is>
-          <t>grapes table</t>
+          <t>blueberries</t>
         </is>
       </c>
       <c r="C145" s="2" t="inlineStr"/>
@@ -2368,7 +2368,7 @@
       <c r="A146" s="2" t="n"/>
       <c r="B146" s="2" t="inlineStr">
         <is>
-          <t>avocados</t>
+          <t>dragon fruit</t>
         </is>
       </c>
       <c r="C146" s="2" t="inlineStr"/>
@@ -2380,7 +2380,7 @@
       <c r="A147" s="2" t="n"/>
       <c r="B147" s="2" t="inlineStr">
         <is>
-          <t>grapes wine</t>
+          <t>grapefruit</t>
         </is>
       </c>
       <c r="C147" s="2" t="inlineStr"/>
@@ -2392,7 +2392,7 @@
       <c r="A148" s="2" t="n"/>
       <c r="B148" s="2" t="inlineStr">
         <is>
-          <t>bananas</t>
+          <t>rambutans</t>
         </is>
       </c>
       <c r="C148" s="2" t="inlineStr"/>
@@ -2404,7 +2404,7 @@
       <c r="A149" s="2" t="n"/>
       <c r="B149" s="2" t="inlineStr">
         <is>
-          <t>loganberries</t>
+          <t>avocados</t>
         </is>
       </c>
       <c r="C149" s="2" t="inlineStr"/>
@@ -2416,7 +2416,7 @@
       <c r="A150" s="2" t="n"/>
       <c r="B150" s="2" t="inlineStr">
         <is>
-          <t>plums</t>
+          <t>strawberries</t>
         </is>
       </c>
       <c r="C150" s="2" t="inlineStr"/>
@@ -2428,7 +2428,7 @@
       <c r="A151" s="2" t="n"/>
       <c r="B151" s="2" t="inlineStr">
         <is>
-          <t>rambutans</t>
+          <t>grapes dried</t>
         </is>
       </c>
       <c r="C151" s="2" t="inlineStr"/>
@@ -2440,7 +2440,7 @@
       <c r="A152" s="2" t="n"/>
       <c r="B152" s="2" t="inlineStr">
         <is>
-          <t>mandarins</t>
+          <t>figs</t>
         </is>
       </c>
       <c r="C152" s="2" t="inlineStr"/>
@@ -2472,7 +2472,7 @@
       </c>
       <c r="B154" s="2" t="inlineStr">
         <is>
-          <t>nickel</t>
+          <t>aluminium</t>
         </is>
       </c>
       <c r="C154" s="2" t="inlineStr"/>
@@ -2484,7 +2484,7 @@
       <c r="A155" s="2" t="n"/>
       <c r="B155" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">coal_brown </t>
+          <t>salt</t>
         </is>
       </c>
       <c r="C155" s="2" t="inlineStr"/>
@@ -2508,7 +2508,7 @@
       <c r="A157" s="2" t="n"/>
       <c r="B157" s="2" t="inlineStr">
         <is>
-          <t>aluminium</t>
+          <t>copper</t>
         </is>
       </c>
       <c r="C157" s="2" t="inlineStr"/>
@@ -2520,7 +2520,7 @@
       <c r="A158" s="2" t="n"/>
       <c r="B158" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">diamonds_rough </t>
+          <t>coal</t>
         </is>
       </c>
       <c r="C158" s="2" t="inlineStr"/>
@@ -2532,7 +2532,7 @@
       <c r="A159" s="2" t="n"/>
       <c r="B159" s="2" t="inlineStr">
         <is>
-          <t>shingle</t>
+          <t>zinc</t>
         </is>
       </c>
       <c r="C159" s="2" t="inlineStr"/>
@@ -2544,7 +2544,7 @@
       <c r="A160" s="2" t="n"/>
       <c r="B160" s="2" t="inlineStr">
         <is>
-          <t>uranium</t>
+          <t xml:space="preserve">coal_black </t>
         </is>
       </c>
       <c r="C160" s="2" t="inlineStr"/>
@@ -2556,7 +2556,7 @@
       <c r="A161" s="2" t="n"/>
       <c r="B161" s="2" t="inlineStr">
         <is>
-          <t>gold</t>
+          <t xml:space="preserve">rare_earths </t>
         </is>
       </c>
       <c r="C161" s="2" t="inlineStr"/>
@@ -2568,7 +2568,7 @@
       <c r="A162" s="2" t="n"/>
       <c r="B162" s="2" t="inlineStr">
         <is>
-          <t>copper</t>
+          <t>iron_ore</t>
         </is>
       </c>
       <c r="C162" s="2" t="inlineStr"/>
@@ -2580,7 +2580,7 @@
       <c r="A163" s="2" t="n"/>
       <c r="B163" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">rare_earths </t>
+          <t>lead</t>
         </is>
       </c>
       <c r="C163" s="2" t="inlineStr"/>
@@ -2592,7 +2592,7 @@
       <c r="A164" s="2" t="n"/>
       <c r="B164" s="2" t="inlineStr">
         <is>
-          <t>salt</t>
+          <t>zeolite</t>
         </is>
       </c>
       <c r="C164" s="2" t="inlineStr"/>
@@ -2604,7 +2604,7 @@
       <c r="A165" s="2" t="n"/>
       <c r="B165" s="2" t="inlineStr">
         <is>
-          <t>alumina</t>
+          <t xml:space="preserve">coal_brown </t>
         </is>
       </c>
       <c r="C165" s="2" t="inlineStr"/>
@@ -2616,7 +2616,7 @@
       <c r="A166" s="2" t="n"/>
       <c r="B166" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">mineral_sands </t>
+          <t>uranium</t>
         </is>
       </c>
       <c r="C166" s="2" t="inlineStr"/>
@@ -2628,7 +2628,7 @@
       <c r="A167" s="2" t="n"/>
       <c r="B167" s="2" t="inlineStr">
         <is>
-          <t>ironsand</t>
+          <t xml:space="preserve">diamonds_rough </t>
         </is>
       </c>
       <c r="C167" s="2" t="inlineStr"/>
@@ -2652,7 +2652,7 @@
       <c r="A169" s="2" t="n"/>
       <c r="B169" s="2" t="inlineStr">
         <is>
-          <t>zinc</t>
+          <t>bauxite</t>
         </is>
       </c>
       <c r="C169" s="2" t="inlineStr"/>
@@ -2664,7 +2664,7 @@
       <c r="A170" s="2" t="n"/>
       <c r="B170" s="2" t="inlineStr">
         <is>
-          <t>coal</t>
+          <t>gold</t>
         </is>
       </c>
       <c r="C170" s="2" t="inlineStr"/>
@@ -2676,7 +2676,7 @@
       <c r="A171" s="2" t="n"/>
       <c r="B171" s="2" t="inlineStr">
         <is>
-          <t>metal</t>
+          <t>alumina</t>
         </is>
       </c>
       <c r="C171" s="2" t="inlineStr"/>
@@ -2688,7 +2688,7 @@
       <c r="A172" s="2" t="n"/>
       <c r="B172" s="2" t="inlineStr">
         <is>
-          <t>bauxite</t>
+          <t>metal</t>
         </is>
       </c>
       <c r="C172" s="2" t="inlineStr"/>
@@ -2700,7 +2700,7 @@
       <c r="A173" s="2" t="n"/>
       <c r="B173" s="2" t="inlineStr">
         <is>
-          <t>zeolite</t>
+          <t>nickel</t>
         </is>
       </c>
       <c r="C173" s="2" t="inlineStr"/>
@@ -2712,7 +2712,7 @@
       <c r="A174" s="2" t="n"/>
       <c r="B174" s="2" t="inlineStr">
         <is>
-          <t>lead</t>
+          <t>shingle</t>
         </is>
       </c>
       <c r="C174" s="2" t="inlineStr"/>
@@ -2724,7 +2724,7 @@
       <c r="A175" s="2" t="n"/>
       <c r="B175" s="2" t="inlineStr">
         <is>
-          <t>iron_ore</t>
+          <t>ironsand</t>
         </is>
       </c>
       <c r="C175" s="2" t="inlineStr"/>
@@ -2736,7 +2736,7 @@
       <c r="A176" s="2" t="n"/>
       <c r="B176" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">coal_black </t>
+          <t xml:space="preserve">mineral_sands </t>
         </is>
       </c>
       <c r="C176" s="2" t="inlineStr"/>
@@ -2752,7 +2752,7 @@
       </c>
       <c r="B177" s="2" t="inlineStr">
         <is>
-          <t>pecan nuts</t>
+          <t>pinenuts</t>
         </is>
       </c>
       <c r="C177" s="2" t="inlineStr"/>
@@ -2764,7 +2764,7 @@
       <c r="A178" s="2" t="n"/>
       <c r="B178" s="2" t="inlineStr">
         <is>
-          <t>chestnuts</t>
+          <t>pecan nuts</t>
         </is>
       </c>
       <c r="C178" s="2" t="inlineStr"/>
@@ -2788,7 +2788,7 @@
       <c r="A180" s="2" t="n"/>
       <c r="B180" s="2" t="inlineStr">
         <is>
-          <t>macadamias</t>
+          <t>cashews</t>
         </is>
       </c>
       <c r="C180" s="2" t="inlineStr"/>
@@ -2800,7 +2800,7 @@
       <c r="A181" s="2" t="n"/>
       <c r="B181" s="2" t="inlineStr">
         <is>
-          <t>hazelnuts</t>
+          <t>macadamias</t>
         </is>
       </c>
       <c r="C181" s="2" t="inlineStr"/>
@@ -2812,7 +2812,7 @@
       <c r="A182" s="2" t="n"/>
       <c r="B182" s="2" t="inlineStr">
         <is>
-          <t>pinenuts</t>
+          <t>brazil nuts</t>
         </is>
       </c>
       <c r="C182" s="2" t="inlineStr"/>
@@ -2836,7 +2836,7 @@
       <c r="A184" s="2" t="n"/>
       <c r="B184" s="2" t="inlineStr">
         <is>
-          <t>cashews</t>
+          <t>pistachios</t>
         </is>
       </c>
       <c r="C184" s="2" t="inlineStr"/>
@@ -2848,7 +2848,7 @@
       <c r="A185" s="2" t="n"/>
       <c r="B185" s="2" t="inlineStr">
         <is>
-          <t>pistachios</t>
+          <t>hazelnuts</t>
         </is>
       </c>
       <c r="C185" s="2" t="inlineStr"/>
@@ -2860,7 +2860,7 @@
       <c r="A186" s="2" t="n"/>
       <c r="B186" s="2" t="inlineStr">
         <is>
-          <t>brazil nuts</t>
+          <t>chestnuts</t>
         </is>
       </c>
       <c r="C186" s="2" t="inlineStr"/>
@@ -2876,7 +2876,7 @@
       </c>
       <c r="B187" s="2" t="inlineStr">
         <is>
-          <t>sesame</t>
+          <t>canola</t>
         </is>
       </c>
       <c r="C187" s="2" t="inlineStr"/>
@@ -2888,7 +2888,7 @@
       <c r="A188" s="2" t="n"/>
       <c r="B188" s="2" t="inlineStr">
         <is>
-          <t>flaxseed</t>
+          <t>soybeans</t>
         </is>
       </c>
       <c r="C188" s="2" t="inlineStr"/>
@@ -2900,7 +2900,7 @@
       <c r="A189" s="2" t="n"/>
       <c r="B189" s="2" t="inlineStr">
         <is>
-          <t>sunflower</t>
+          <t xml:space="preserve">mustard </t>
         </is>
       </c>
       <c r="C189" s="2" t="inlineStr"/>
@@ -2912,7 +2912,7 @@
       <c r="A190" s="2" t="n"/>
       <c r="B190" s="2" t="inlineStr">
         <is>
-          <t>canola</t>
+          <t>sunflower</t>
         </is>
       </c>
       <c r="C190" s="2" t="inlineStr"/>
@@ -2924,7 +2924,7 @@
       <c r="A191" s="2" t="n"/>
       <c r="B191" s="2" t="inlineStr">
         <is>
-          <t>safflower</t>
+          <t>chia</t>
         </is>
       </c>
       <c r="C191" s="2" t="inlineStr"/>
@@ -2936,7 +2936,7 @@
       <c r="A192" s="2" t="n"/>
       <c r="B192" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">mustard </t>
+          <t>safflower</t>
         </is>
       </c>
       <c r="C192" s="2" t="inlineStr"/>
@@ -2948,7 +2948,7 @@
       <c r="A193" s="2" t="n"/>
       <c r="B193" s="2" t="inlineStr">
         <is>
-          <t>soybeans</t>
+          <t>sesame</t>
         </is>
       </c>
       <c r="C193" s="2" t="inlineStr"/>
@@ -2960,7 +2960,7 @@
       <c r="A194" s="2" t="n"/>
       <c r="B194" s="2" t="inlineStr">
         <is>
-          <t>chia</t>
+          <t>peanuts</t>
         </is>
       </c>
       <c r="C194" s="2" t="inlineStr"/>
@@ -2972,7 +2972,7 @@
       <c r="A195" s="2" t="n"/>
       <c r="B195" s="2" t="inlineStr">
         <is>
-          <t>peanuts</t>
+          <t>flaxseed</t>
         </is>
       </c>
       <c r="C195" s="2" t="inlineStr"/>
@@ -3012,7 +3012,7 @@
       <c r="A198" s="2" t="n"/>
       <c r="B198" s="2" t="inlineStr">
         <is>
-          <t>lucerne</t>
+          <t>turnips forage</t>
         </is>
       </c>
       <c r="C198" s="2" t="inlineStr"/>
@@ -3024,7 +3024,7 @@
       <c r="A199" s="2" t="n"/>
       <c r="B199" s="2" t="inlineStr">
         <is>
-          <t>clover</t>
+          <t>lucerne</t>
         </is>
       </c>
       <c r="C199" s="2" t="inlineStr"/>
@@ -3036,7 +3036,7 @@
       <c r="A200" s="2" t="n"/>
       <c r="B200" s="2" t="inlineStr">
         <is>
-          <t>turnips forage</t>
+          <t>plantain</t>
         </is>
       </c>
       <c r="C200" s="2" t="inlineStr"/>
@@ -3048,7 +3048,7 @@
       <c r="A201" s="2" t="n"/>
       <c r="B201" s="2" t="inlineStr">
         <is>
-          <t>plantain</t>
+          <t>clover</t>
         </is>
       </c>
       <c r="C201" s="2" t="inlineStr"/>
@@ -3064,7 +3064,7 @@
       </c>
       <c r="B202" s="2" t="inlineStr">
         <is>
-          <t>chickpeas</t>
+          <t>navy bean</t>
         </is>
       </c>
       <c r="C202" s="2" t="inlineStr"/>
@@ -3076,7 +3076,7 @@
       <c r="A203" s="2" t="n"/>
       <c r="B203" s="2" t="inlineStr">
         <is>
-          <t>lentils</t>
+          <t>azuki bean</t>
         </is>
       </c>
       <c r="C203" s="2" t="inlineStr"/>
@@ -3088,7 +3088,7 @@
       <c r="A204" s="2" t="n"/>
       <c r="B204" s="2" t="inlineStr">
         <is>
-          <t>navy bean</t>
+          <t>lupins</t>
         </is>
       </c>
       <c r="C204" s="2" t="inlineStr"/>
@@ -3112,7 +3112,7 @@
       <c r="A206" s="2" t="n"/>
       <c r="B206" s="2" t="inlineStr">
         <is>
-          <t>broad beans</t>
+          <t>field beans</t>
         </is>
       </c>
       <c r="C206" s="2" t="inlineStr"/>
@@ -3124,7 +3124,7 @@
       <c r="A207" s="2" t="n"/>
       <c r="B207" s="2" t="inlineStr">
         <is>
-          <t>pigeon pea</t>
+          <t>lentils</t>
         </is>
       </c>
       <c r="C207" s="2" t="inlineStr"/>
@@ -3134,11 +3134,7 @@
     </row>
     <row r="208">
       <c r="A208" s="2" t="n"/>
-      <c r="B208" s="2" t="inlineStr">
-        <is>
-          <t>field peas</t>
-        </is>
-      </c>
+      <c r="B208" s="2" t="inlineStr"/>
       <c r="C208" s="2" t="inlineStr"/>
       <c r="D208" s="2" t="inlineStr"/>
       <c r="E208" s="2" t="inlineStr"/>
@@ -3148,7 +3144,7 @@
       <c r="A209" s="2" t="n"/>
       <c r="B209" s="2" t="inlineStr">
         <is>
-          <t>cowpea</t>
+          <t>broad beans</t>
         </is>
       </c>
       <c r="C209" s="2" t="inlineStr"/>
@@ -3160,7 +3156,7 @@
       <c r="A210" s="2" t="n"/>
       <c r="B210" s="2" t="inlineStr">
         <is>
-          <t>field beans</t>
+          <t>chickpeas</t>
         </is>
       </c>
       <c r="C210" s="2" t="inlineStr"/>
@@ -3172,7 +3168,7 @@
       <c r="A211" s="2" t="n"/>
       <c r="B211" s="2" t="inlineStr">
         <is>
-          <t>azuki bean</t>
+          <t>cowpea</t>
         </is>
       </c>
       <c r="C211" s="2" t="inlineStr"/>
@@ -3182,7 +3178,11 @@
     </row>
     <row r="212">
       <c r="A212" s="2" t="n"/>
-      <c r="B212" s="2" t="inlineStr"/>
+      <c r="B212" s="2" t="inlineStr">
+        <is>
+          <t>pigeon pea</t>
+        </is>
+      </c>
       <c r="C212" s="2" t="inlineStr"/>
       <c r="D212" s="2" t="inlineStr"/>
       <c r="E212" s="2" t="inlineStr"/>
@@ -3192,7 +3192,7 @@
       <c r="A213" s="2" t="n"/>
       <c r="B213" s="2" t="inlineStr">
         <is>
-          <t>lupins</t>
+          <t>field peas</t>
         </is>
       </c>
       <c r="C213" s="2" t="inlineStr"/>
@@ -3208,7 +3208,7 @@
       </c>
       <c r="B214" s="2" t="inlineStr">
         <is>
-          <t>sprouts</t>
+          <t>eggplants</t>
         </is>
       </c>
       <c r="C214" s="2" t="inlineStr"/>
@@ -3220,7 +3220,7 @@
       <c r="A215" s="2" t="n"/>
       <c r="B215" s="2" t="inlineStr">
         <is>
-          <t>chervil</t>
+          <t>carrots</t>
         </is>
       </c>
       <c r="C215" s="2" t="inlineStr"/>
@@ -3232,7 +3232,7 @@
       <c r="A216" s="2" t="n"/>
       <c r="B216" s="2" t="inlineStr">
         <is>
-          <t>chinese cabbages</t>
+          <t>arrowroot</t>
         </is>
       </c>
       <c r="C216" s="2" t="inlineStr"/>
@@ -3244,7 +3244,7 @@
       <c r="A217" s="2" t="n"/>
       <c r="B217" s="2" t="inlineStr">
         <is>
-          <t>chicory</t>
+          <t>pumpkins</t>
         </is>
       </c>
       <c r="C217" s="2" t="inlineStr"/>
@@ -3256,7 +3256,7 @@
       <c r="A218" s="2" t="n"/>
       <c r="B218" s="2" t="inlineStr">
         <is>
-          <t>tomatoes</t>
+          <t>rocket</t>
         </is>
       </c>
       <c r="C218" s="2" t="inlineStr"/>
@@ -3268,7 +3268,7 @@
       <c r="A219" s="2" t="n"/>
       <c r="B219" s="2" t="inlineStr">
         <is>
-          <t>peas</t>
+          <t>burdock</t>
         </is>
       </c>
       <c r="C219" s="2" t="inlineStr"/>
@@ -3280,7 +3280,7 @@
       <c r="A220" s="2" t="n"/>
       <c r="B220" s="2" t="inlineStr">
         <is>
-          <t>peppermint</t>
+          <t>sweet corn</t>
         </is>
       </c>
       <c r="C220" s="2" t="inlineStr"/>
@@ -3292,7 +3292,7 @@
       <c r="A221" s="2" t="n"/>
       <c r="B221" s="2" t="inlineStr">
         <is>
-          <t>burdock</t>
+          <t>radishes</t>
         </is>
       </c>
       <c r="C221" s="2" t="inlineStr"/>
@@ -3304,7 +3304,7 @@
       <c r="A222" s="2" t="n"/>
       <c r="B222" s="2" t="inlineStr">
         <is>
-          <t>onions</t>
+          <t>sage</t>
         </is>
       </c>
       <c r="C222" s="2" t="inlineStr"/>
@@ -3316,7 +3316,7 @@
       <c r="A223" s="2" t="n"/>
       <c r="B223" s="2" t="inlineStr">
         <is>
-          <t>oregano</t>
+          <t>chicory</t>
         </is>
       </c>
       <c r="C223" s="2" t="inlineStr"/>
@@ -3328,7 +3328,7 @@
       <c r="A224" s="2" t="n"/>
       <c r="B224" s="2" t="inlineStr">
         <is>
-          <t>swedes</t>
+          <t>rosemary</t>
         </is>
       </c>
       <c r="C224" s="2" t="inlineStr"/>
@@ -3340,7 +3340,7 @@
       <c r="A225" s="2" t="n"/>
       <c r="B225" s="2" t="inlineStr">
         <is>
-          <t>vegetables</t>
+          <t>marjoram</t>
         </is>
       </c>
       <c r="C225" s="2" t="inlineStr"/>
@@ -3352,7 +3352,7 @@
       <c r="A226" s="2" t="n"/>
       <c r="B226" s="2" t="inlineStr">
         <is>
-          <t>capsicums</t>
+          <t>parsnips</t>
         </is>
       </c>
       <c r="C226" s="2" t="inlineStr"/>
@@ -3364,7 +3364,7 @@
       <c r="A227" s="2" t="n"/>
       <c r="B227" s="2" t="inlineStr">
         <is>
-          <t>kale</t>
+          <t>chives</t>
         </is>
       </c>
       <c r="C227" s="2" t="inlineStr"/>
@@ -3376,7 +3376,7 @@
       <c r="A228" s="2" t="n"/>
       <c r="B228" s="2" t="inlineStr">
         <is>
-          <t>mushrooms</t>
+          <t>okra</t>
         </is>
       </c>
       <c r="C228" s="2" t="inlineStr"/>
@@ -3388,7 +3388,7 @@
       <c r="A229" s="2" t="n"/>
       <c r="B229" s="2" t="inlineStr">
         <is>
-          <t>beetroot</t>
+          <t>artichokes</t>
         </is>
       </c>
       <c r="C229" s="2" t="inlineStr"/>
@@ -3400,7 +3400,7 @@
       <c r="A230" s="2" t="n"/>
       <c r="B230" s="2" t="inlineStr">
         <is>
-          <t>potatoes</t>
+          <t>broccoli</t>
         </is>
       </c>
       <c r="C230" s="2" t="inlineStr"/>
@@ -3412,7 +3412,7 @@
       <c r="A231" s="2" t="n"/>
       <c r="B231" s="2" t="inlineStr">
         <is>
-          <t>truffles</t>
+          <t>cauliflowers</t>
         </is>
       </c>
       <c r="C231" s="2" t="inlineStr"/>
@@ -3424,7 +3424,7 @@
       <c r="A232" s="2" t="n"/>
       <c r="B232" s="2" t="inlineStr">
         <is>
-          <t>lettuces</t>
+          <t>cucumbers</t>
         </is>
       </c>
       <c r="C232" s="2" t="inlineStr"/>
@@ -3436,7 +3436,7 @@
       <c r="A233" s="2" t="n"/>
       <c r="B233" s="2" t="inlineStr">
         <is>
-          <t>cauliflowers</t>
+          <t>kale</t>
         </is>
       </c>
       <c r="C233" s="2" t="inlineStr"/>
@@ -3448,7 +3448,7 @@
       <c r="A234" s="2" t="n"/>
       <c r="B234" s="2" t="inlineStr">
         <is>
-          <t>coriander</t>
+          <t>thyme</t>
         </is>
       </c>
       <c r="C234" s="2" t="inlineStr"/>
@@ -3460,7 +3460,7 @@
       <c r="A235" s="2" t="n"/>
       <c r="B235" s="2" t="inlineStr">
         <is>
-          <t>lemongrass</t>
+          <t>celery</t>
         </is>
       </c>
       <c r="C235" s="2" t="inlineStr"/>
@@ -3472,7 +3472,7 @@
       <c r="A236" s="2" t="n"/>
       <c r="B236" s="2" t="inlineStr">
         <is>
-          <t>silverbeet and spinach</t>
+          <t>onions</t>
         </is>
       </c>
       <c r="C236" s="2" t="inlineStr"/>
@@ -3484,7 +3484,7 @@
       <c r="A237" s="2" t="n"/>
       <c r="B237" s="2" t="inlineStr">
         <is>
-          <t>brussels sprouts</t>
+          <t>turnips</t>
         </is>
       </c>
       <c r="C237" s="2" t="inlineStr"/>
@@ -3496,7 +3496,7 @@
       <c r="A238" s="2" t="n"/>
       <c r="B238" s="2" t="inlineStr">
         <is>
-          <t>arrowroot</t>
+          <t>lettuces</t>
         </is>
       </c>
       <c r="C238" s="2" t="inlineStr"/>
@@ -3508,7 +3508,7 @@
       <c r="A239" s="2" t="n"/>
       <c r="B239" s="2" t="inlineStr">
         <is>
-          <t>rosemary</t>
+          <t>peas</t>
         </is>
       </c>
       <c r="C239" s="2" t="inlineStr"/>
@@ -3520,7 +3520,7 @@
       <c r="A240" s="2" t="n"/>
       <c r="B240" s="2" t="inlineStr">
         <is>
-          <t>gherkins</t>
+          <t>swedes</t>
         </is>
       </c>
       <c r="C240" s="2" t="inlineStr"/>
@@ -3532,7 +3532,7 @@
       <c r="A241" s="2" t="n"/>
       <c r="B241" s="2" t="inlineStr">
         <is>
-          <t>kumara</t>
+          <t>cabbages</t>
         </is>
       </c>
       <c r="C241" s="2" t="inlineStr"/>
@@ -3544,7 +3544,7 @@
       <c r="A242" s="2" t="n"/>
       <c r="B242" s="2" t="inlineStr">
         <is>
-          <t>fennel</t>
+          <t>kumara</t>
         </is>
       </c>
       <c r="C242" s="2" t="inlineStr"/>
@@ -3556,7 +3556,7 @@
       <c r="A243" s="2" t="n"/>
       <c r="B243" s="2" t="inlineStr">
         <is>
-          <t>snowpeas</t>
+          <t>echinacea</t>
         </is>
       </c>
       <c r="C243" s="2" t="inlineStr"/>
@@ -3568,7 +3568,7 @@
       <c r="A244" s="2" t="n"/>
       <c r="B244" s="2" t="inlineStr">
         <is>
-          <t>zucchini</t>
+          <t>oregano</t>
         </is>
       </c>
       <c r="C244" s="2" t="inlineStr"/>
@@ -3580,7 +3580,7 @@
       <c r="A245" s="2" t="n"/>
       <c r="B245" s="2" t="inlineStr">
         <is>
-          <t>rocket</t>
+          <t>sugar beet</t>
         </is>
       </c>
       <c r="C245" s="2" t="inlineStr"/>
@@ -3592,7 +3592,7 @@
       <c r="A246" s="2" t="n"/>
       <c r="B246" s="2" t="inlineStr">
         <is>
-          <t>celery</t>
+          <t>capsicums</t>
         </is>
       </c>
       <c r="C246" s="2" t="inlineStr"/>
@@ -3604,7 +3604,7 @@
       <c r="A247" s="2" t="n"/>
       <c r="B247" s="2" t="inlineStr">
         <is>
-          <t>parsnips</t>
+          <t>chillies</t>
         </is>
       </c>
       <c r="C247" s="2" t="inlineStr"/>
@@ -3616,7 +3616,7 @@
       <c r="A248" s="2" t="n"/>
       <c r="B248" s="2" t="inlineStr">
         <is>
-          <t>marrows and squashes</t>
+          <t>truffles</t>
         </is>
       </c>
       <c r="C248" s="2" t="inlineStr"/>
@@ -3628,7 +3628,7 @@
       <c r="A249" s="2" t="n"/>
       <c r="B249" s="2" t="inlineStr">
         <is>
-          <t>turnips</t>
+          <t>silverbeet and spinach</t>
         </is>
       </c>
       <c r="C249" s="2" t="inlineStr"/>
@@ -3640,7 +3640,7 @@
       <c r="A250" s="2" t="n"/>
       <c r="B250" s="2" t="inlineStr">
         <is>
-          <t>marjoram</t>
+          <t>french beans</t>
         </is>
       </c>
       <c r="C250" s="2" t="inlineStr"/>
@@ -3652,7 +3652,7 @@
       <c r="A251" s="2" t="n"/>
       <c r="B251" s="2" t="inlineStr">
         <is>
-          <t>garlic</t>
+          <t>sweet potatoes</t>
         </is>
       </c>
       <c r="C251" s="2" t="inlineStr"/>
@@ -3664,7 +3664,7 @@
       <c r="A252" s="2" t="n"/>
       <c r="B252" s="2" t="inlineStr">
         <is>
-          <t>vegetable seeds</t>
+          <t>tomatoes</t>
         </is>
       </c>
       <c r="C252" s="2" t="inlineStr"/>
@@ -3676,7 +3676,7 @@
       <c r="A253" s="2" t="n"/>
       <c r="B253" s="2" t="inlineStr">
         <is>
-          <t>chillies</t>
+          <t>rhubarb</t>
         </is>
       </c>
       <c r="C253" s="2" t="inlineStr"/>
@@ -3688,7 +3688,7 @@
       <c r="A254" s="2" t="n"/>
       <c r="B254" s="2" t="inlineStr">
         <is>
-          <t>mint</t>
+          <t>vegetables</t>
         </is>
       </c>
       <c r="C254" s="2" t="inlineStr"/>
@@ -3700,7 +3700,7 @@
       <c r="A255" s="2" t="n"/>
       <c r="B255" s="2" t="inlineStr">
         <is>
-          <t>tarragon</t>
+          <t>snowpeas</t>
         </is>
       </c>
       <c r="C255" s="2" t="inlineStr"/>
@@ -3712,7 +3712,7 @@
       <c r="A256" s="2" t="n"/>
       <c r="B256" s="2" t="inlineStr">
         <is>
-          <t>chamomile</t>
+          <t>coriander</t>
         </is>
       </c>
       <c r="C256" s="2" t="inlineStr"/>
@@ -3724,7 +3724,7 @@
       <c r="A257" s="2" t="n"/>
       <c r="B257" s="2" t="inlineStr">
         <is>
-          <t>eggplants</t>
+          <t>tarragon</t>
         </is>
       </c>
       <c r="C257" s="2" t="inlineStr"/>
@@ -3736,7 +3736,7 @@
       <c r="A258" s="2" t="n"/>
       <c r="B258" s="2" t="inlineStr">
         <is>
-          <t>herbs</t>
+          <t>zucchini</t>
         </is>
       </c>
       <c r="C258" s="2" t="inlineStr"/>
@@ -3748,7 +3748,7 @@
       <c r="A259" s="2" t="n"/>
       <c r="B259" s="2" t="inlineStr">
         <is>
-          <t>sage</t>
+          <t>herbs</t>
         </is>
       </c>
       <c r="C259" s="2" t="inlineStr"/>
@@ -3760,7 +3760,7 @@
       <c r="A260" s="2" t="n"/>
       <c r="B260" s="2" t="inlineStr">
         <is>
-          <t>radishes</t>
+          <t>mushrooms</t>
         </is>
       </c>
       <c r="C260" s="2" t="inlineStr"/>
@@ -3772,7 +3772,7 @@
       <c r="A261" s="2" t="n"/>
       <c r="B261" s="2" t="inlineStr">
         <is>
-          <t>rhubarb</t>
+          <t>gherkins</t>
         </is>
       </c>
       <c r="C261" s="2" t="inlineStr"/>
@@ -3784,7 +3784,7 @@
       <c r="A262" s="2" t="n"/>
       <c r="B262" s="2" t="inlineStr">
         <is>
-          <t>cucumbers</t>
+          <t>marrows and squashes</t>
         </is>
       </c>
       <c r="C262" s="2" t="inlineStr"/>
@@ -3796,7 +3796,7 @@
       <c r="A263" s="2" t="n"/>
       <c r="B263" s="2" t="inlineStr">
         <is>
-          <t>parsley</t>
+          <t>lemongrass</t>
         </is>
       </c>
       <c r="C263" s="2" t="inlineStr"/>
@@ -3808,7 +3808,7 @@
       <c r="A264" s="2" t="n"/>
       <c r="B264" s="2" t="inlineStr">
         <is>
-          <t>pumpkins</t>
+          <t>potatoes</t>
         </is>
       </c>
       <c r="C264" s="2" t="inlineStr"/>
@@ -3820,7 +3820,7 @@
       <c r="A265" s="2" t="n"/>
       <c r="B265" s="2" t="inlineStr">
         <is>
-          <t>sugar beet</t>
+          <t>spring onions and shallots</t>
         </is>
       </c>
       <c r="C265" s="2" t="inlineStr"/>
@@ -3832,7 +3832,7 @@
       <c r="A266" s="2" t="n"/>
       <c r="B266" s="2" t="inlineStr">
         <is>
-          <t>cabbages</t>
+          <t>leeks</t>
         </is>
       </c>
       <c r="C266" s="2" t="inlineStr"/>
@@ -3844,7 +3844,7 @@
       <c r="A267" s="2" t="n"/>
       <c r="B267" s="2" t="inlineStr">
         <is>
-          <t>leeks</t>
+          <t>beetroot</t>
         </is>
       </c>
       <c r="C267" s="2" t="inlineStr"/>
@@ -3856,7 +3856,7 @@
       <c r="A268" s="2" t="n"/>
       <c r="B268" s="2" t="inlineStr">
         <is>
-          <t>spring onions and shallots</t>
+          <t>asparagus</t>
         </is>
       </c>
       <c r="C268" s="2" t="inlineStr"/>
@@ -3868,7 +3868,7 @@
       <c r="A269" s="2" t="n"/>
       <c r="B269" s="2" t="inlineStr">
         <is>
-          <t>okra</t>
+          <t>bitter melon</t>
         </is>
       </c>
       <c r="C269" s="2" t="inlineStr"/>
@@ -3880,7 +3880,7 @@
       <c r="A270" s="2" t="n"/>
       <c r="B270" s="2" t="inlineStr">
         <is>
-          <t>asparagus</t>
+          <t>garlic</t>
         </is>
       </c>
       <c r="C270" s="2" t="inlineStr"/>
@@ -3892,7 +3892,7 @@
       <c r="A271" s="2" t="n"/>
       <c r="B271" s="2" t="inlineStr">
         <is>
-          <t>sweet potatoes</t>
+          <t>peppermint</t>
         </is>
       </c>
       <c r="C271" s="2" t="inlineStr"/>
@@ -3904,7 +3904,7 @@
       <c r="A272" s="2" t="n"/>
       <c r="B272" s="2" t="inlineStr">
         <is>
-          <t>beans</t>
+          <t>mint</t>
         </is>
       </c>
       <c r="C272" s="2" t="inlineStr"/>
@@ -3916,7 +3916,7 @@
       <c r="A273" s="2" t="n"/>
       <c r="B273" s="2" t="inlineStr">
         <is>
-          <t>artichokes</t>
+          <t>vegetable seeds</t>
         </is>
       </c>
       <c r="C273" s="2" t="inlineStr"/>
@@ -3928,7 +3928,7 @@
       <c r="A274" s="2" t="n"/>
       <c r="B274" s="2" t="inlineStr">
         <is>
-          <t>bitter melon</t>
+          <t>sprouts</t>
         </is>
       </c>
       <c r="C274" s="2" t="inlineStr"/>
@@ -3940,7 +3940,7 @@
       <c r="A275" s="2" t="n"/>
       <c r="B275" s="2" t="inlineStr">
         <is>
-          <t>broccoli</t>
+          <t>parsley</t>
         </is>
       </c>
       <c r="C275" s="2" t="inlineStr"/>
@@ -3952,7 +3952,7 @@
       <c r="A276" s="2" t="n"/>
       <c r="B276" s="2" t="inlineStr">
         <is>
-          <t>chives</t>
+          <t>chamomile</t>
         </is>
       </c>
       <c r="C276" s="2" t="inlineStr"/>
@@ -3964,7 +3964,7 @@
       <c r="A277" s="2" t="n"/>
       <c r="B277" s="2" t="inlineStr">
         <is>
-          <t>thyme</t>
+          <t>fennel</t>
         </is>
       </c>
       <c r="C277" s="2" t="inlineStr"/>
@@ -3976,7 +3976,7 @@
       <c r="A278" s="2" t="n"/>
       <c r="B278" s="2" t="inlineStr">
         <is>
-          <t>carrots</t>
+          <t>beans</t>
         </is>
       </c>
       <c r="C278" s="2" t="inlineStr"/>
@@ -3988,7 +3988,7 @@
       <c r="A279" s="2" t="n"/>
       <c r="B279" s="2" t="inlineStr">
         <is>
-          <t>echinacea</t>
+          <t>chinese cabbages</t>
         </is>
       </c>
       <c r="C279" s="2" t="inlineStr"/>
@@ -4000,7 +4000,7 @@
       <c r="A280" s="2" t="n"/>
       <c r="B280" s="2" t="inlineStr">
         <is>
-          <t>sweet corn</t>
+          <t>brussels sprouts</t>
         </is>
       </c>
       <c r="C280" s="2" t="inlineStr"/>
@@ -4012,7 +4012,7 @@
       <c r="A281" s="2" t="n"/>
       <c r="B281" s="2" t="inlineStr">
         <is>
-          <t>french beans</t>
+          <t>chervil</t>
         </is>
       </c>
       <c r="C281" s="2" t="inlineStr"/>

</xml_diff>

<commit_message>
sort by notation, not label, for collections
</commit_message>
<xml_diff>
--- a/classification-systems/nzlum/build/commodities.xlsx
+++ b/classification-systems/nzlum/build/commodities.xlsx
@@ -484,30 +484,26 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>sheep meat</t>
+          <t>bees</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr"/>
       <c r="D2" s="2" t="inlineStr"/>
-      <c r="E2" s="2" t="inlineStr">
-        <is>
-          <t>Sheep for meat production.</t>
-        </is>
-      </c>
+      <c r="E2" s="2" t="inlineStr"/>
       <c r="F2" s="2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n"/>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>cattle dairy</t>
+          <t>cats</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr"/>
       <c r="D3" s="2" t="inlineStr"/>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>Cattle for milk production.</t>
+          <t>Includes cat breeding, catteries, or areas used for quarantine of cats related to import or export.</t>
         </is>
       </c>
       <c r="F3" s="2" t="inlineStr"/>
@@ -516,30 +512,26 @@
       <c r="A4" s="2" t="n"/>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>sheep stud</t>
+          <t>cattle</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr"/>
       <c r="D4" s="2" t="inlineStr"/>
-      <c r="E4" s="2" t="inlineStr">
-        <is>
-          <t>Sheep raised for sale as breeding animals.</t>
-        </is>
-      </c>
+      <c r="E4" s="2" t="inlineStr"/>
       <c r="F4" s="2" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n"/>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>molluscs</t>
+          <t>cattle dairy</t>
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr"/>
       <c r="D5" s="2" t="inlineStr"/>
       <c r="E5" s="2" t="inlineStr">
         <is>
-          <t>Aquaculture: includes peal oysters, edible oysters, abalone, mussels.</t>
+          <t>Cattle for milk production.</t>
         </is>
       </c>
       <c r="F5" s="2" t="inlineStr"/>
@@ -548,14 +540,14 @@
       <c r="A6" s="2" t="n"/>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>finfish</t>
+          <t>cattle meat</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr"/>
       <c r="D6" s="2" t="inlineStr"/>
       <c r="E6" s="2" t="inlineStr">
         <is>
-          <t>Aquaculture: tuna, salmon, trout, freshwater species, etc.</t>
+          <t>Cattle for meat (beef) production.</t>
         </is>
       </c>
       <c r="F6" s="2" t="inlineStr"/>
@@ -564,50 +556,62 @@
       <c r="A7" s="2" t="n"/>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>bees</t>
+          <t>cattle stud</t>
         </is>
       </c>
       <c r="C7" s="2" t="inlineStr"/>
       <c r="D7" s="2" t="inlineStr"/>
-      <c r="E7" s="2" t="inlineStr"/>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>Cattle raised for sale as breeding animals.</t>
+        </is>
+      </c>
       <c r="F7" s="2" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n"/>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>deer</t>
+          <t>chickens</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr"/>
       <c r="D8" s="2" t="inlineStr"/>
-      <c r="E8" s="2" t="inlineStr"/>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>Poultry farms. Specify whether for eggs or meat where possible.</t>
+        </is>
+      </c>
       <c r="F8" s="2" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n"/>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>cattle</t>
+          <t>chickens eggs</t>
         </is>
       </c>
       <c r="C9" s="2" t="inlineStr"/>
       <c r="D9" s="2" t="inlineStr"/>
-      <c r="E9" s="2" t="inlineStr"/>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>Poultry farms. Production mainly for eggs.</t>
+        </is>
+      </c>
       <c r="F9" s="2" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n"/>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>crustaceans</t>
+          <t>chickens meat</t>
         </is>
       </c>
       <c r="C10" s="2" t="inlineStr"/>
       <c r="D10" s="2" t="inlineStr"/>
       <c r="E10" s="2" t="inlineStr">
         <is>
-          <t>Aquaculture: prawns, freshwater crayfish, etc.</t>
+          <t>Poultry farms. Production mainly for meat.</t>
         </is>
       </c>
       <c r="F10" s="2" t="inlineStr"/>
@@ -616,14 +620,14 @@
       <c r="A11" s="2" t="n"/>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>sheep dairy</t>
+          <t>crocodiles</t>
         </is>
       </c>
       <c r="C11" s="2" t="inlineStr"/>
       <c r="D11" s="2" t="inlineStr"/>
       <c r="E11" s="2" t="inlineStr">
         <is>
-          <t>Sheep for milk production.</t>
+          <t>Aquaculture.</t>
         </is>
       </c>
       <c r="F11" s="2" t="inlineStr"/>
@@ -632,14 +636,14 @@
       <c r="A12" s="2" t="n"/>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>ostriches</t>
+          <t>crustaceans</t>
         </is>
       </c>
       <c r="C12" s="2" t="inlineStr"/>
       <c r="D12" s="2" t="inlineStr"/>
       <c r="E12" s="2" t="inlineStr">
         <is>
-          <t>Poultry farming.</t>
+          <t>Aquaculture: prawns, freshwater crayfish, etc.</t>
         </is>
       </c>
       <c r="F12" s="2" t="inlineStr"/>
@@ -648,30 +652,26 @@
       <c r="A13" s="2" t="n"/>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>cattle meat</t>
+          <t>deer</t>
         </is>
       </c>
       <c r="C13" s="2" t="inlineStr"/>
       <c r="D13" s="2" t="inlineStr"/>
-      <c r="E13" s="2" t="inlineStr">
-        <is>
-          <t>Cattle for meat (beef) production.</t>
-        </is>
-      </c>
+      <c r="E13" s="2" t="inlineStr"/>
       <c r="F13" s="2" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n"/>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>sheep wool</t>
+          <t>dogs</t>
         </is>
       </c>
       <c r="C14" s="2" t="inlineStr"/>
       <c r="D14" s="2" t="inlineStr"/>
       <c r="E14" s="2" t="inlineStr">
         <is>
-          <t>Sheep for fibre production.</t>
+          <t>Includes dog breeding, kennels, or areas used for quarantine of dogs related to import or export.</t>
         </is>
       </c>
       <c r="F14" s="2" t="inlineStr"/>
@@ -680,7 +680,7 @@
       <c r="A15" s="2" t="n"/>
       <c r="B15" s="2" t="inlineStr">
         <is>
-          <t>turkeys</t>
+          <t>ducks</t>
         </is>
       </c>
       <c r="C15" s="2" t="inlineStr"/>
@@ -696,14 +696,14 @@
       <c r="A16" s="2" t="n"/>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>chickens eggs</t>
+          <t>emus</t>
         </is>
       </c>
       <c r="C16" s="2" t="inlineStr"/>
       <c r="D16" s="2" t="inlineStr"/>
       <c r="E16" s="2" t="inlineStr">
         <is>
-          <t>Poultry farms. Production mainly for eggs.</t>
+          <t>Poultry farms.</t>
         </is>
       </c>
       <c r="F16" s="2" t="inlineStr"/>
@@ -712,14 +712,14 @@
       <c r="A17" s="2" t="n"/>
       <c r="B17" s="2" t="inlineStr">
         <is>
-          <t>goats stud</t>
+          <t>finfish</t>
         </is>
       </c>
       <c r="C17" s="2" t="inlineStr"/>
       <c r="D17" s="2" t="inlineStr"/>
       <c r="E17" s="2" t="inlineStr">
         <is>
-          <t>Goats raised for sale as breeding animals.</t>
+          <t>Aquaculture: tuna, salmon, trout, freshwater species, etc.</t>
         </is>
       </c>
       <c r="F17" s="2" t="inlineStr"/>
@@ -728,14 +728,14 @@
       <c r="A18" s="2" t="n"/>
       <c r="B18" s="2" t="inlineStr">
         <is>
-          <t>goats</t>
+          <t>geese</t>
         </is>
       </c>
       <c r="C18" s="2" t="inlineStr"/>
       <c r="D18" s="2" t="inlineStr"/>
       <c r="E18" s="2" t="inlineStr">
         <is>
-          <t>Specify meat, dairy, stud, or wool where appropriate.</t>
+          <t>Poultry farms.</t>
         </is>
       </c>
       <c r="F18" s="2" t="inlineStr"/>
@@ -744,14 +744,14 @@
       <c r="A19" s="2" t="n"/>
       <c r="B19" s="2" t="inlineStr">
         <is>
-          <t>goats wool</t>
+          <t>goats</t>
         </is>
       </c>
       <c r="C19" s="2" t="inlineStr"/>
       <c r="D19" s="2" t="inlineStr"/>
       <c r="E19" s="2" t="inlineStr">
         <is>
-          <t>Goats for fibre production.</t>
+          <t>Specify meat, dairy, stud, or wool where appropriate.</t>
         </is>
       </c>
       <c r="F19" s="2" t="inlineStr"/>
@@ -760,14 +760,14 @@
       <c r="A20" s="2" t="n"/>
       <c r="B20" s="2" t="inlineStr">
         <is>
-          <t>cats</t>
+          <t>goats dairy</t>
         </is>
       </c>
       <c r="C20" s="2" t="inlineStr"/>
       <c r="D20" s="2" t="inlineStr"/>
       <c r="E20" s="2" t="inlineStr">
         <is>
-          <t>Includes cat breeding, catteries, or areas used for quarantine of cats related to import or export.</t>
+          <t>Goats for milk production.</t>
         </is>
       </c>
       <c r="F20" s="2" t="inlineStr"/>
@@ -776,14 +776,14 @@
       <c r="A21" s="2" t="n"/>
       <c r="B21" s="2" t="inlineStr">
         <is>
-          <t>pigs</t>
+          <t>goats meat</t>
         </is>
       </c>
       <c r="C21" s="2" t="inlineStr"/>
       <c r="D21" s="2" t="inlineStr"/>
       <c r="E21" s="2" t="inlineStr">
         <is>
-          <t>Piggeries.</t>
+          <t>Goats for meat production.</t>
         </is>
       </c>
       <c r="F21" s="2" t="inlineStr"/>
@@ -792,14 +792,14 @@
       <c r="A22" s="2" t="n"/>
       <c r="B22" s="2" t="inlineStr">
         <is>
-          <t>sheep</t>
+          <t>goats stud</t>
         </is>
       </c>
       <c r="C22" s="2" t="inlineStr"/>
       <c r="D22" s="2" t="inlineStr"/>
       <c r="E22" s="2" t="inlineStr">
         <is>
-          <t>Specify meat, dairy, stud or wool where appropriate.</t>
+          <t>Goats raised for sale as breeding animals.</t>
         </is>
       </c>
       <c r="F22" s="2" t="inlineStr"/>
@@ -808,14 +808,14 @@
       <c r="A23" s="2" t="n"/>
       <c r="B23" s="2" t="inlineStr">
         <is>
-          <t>crocodiles</t>
+          <t>goats wool</t>
         </is>
       </c>
       <c r="C23" s="2" t="inlineStr"/>
       <c r="D23" s="2" t="inlineStr"/>
       <c r="E23" s="2" t="inlineStr">
         <is>
-          <t>Aquaculture.</t>
+          <t>Goats for fibre production.</t>
         </is>
       </c>
       <c r="F23" s="2" t="inlineStr"/>
@@ -840,14 +840,14 @@
       <c r="A25" s="2" t="n"/>
       <c r="B25" s="2" t="inlineStr">
         <is>
-          <t>cattle stud</t>
+          <t>molluscs</t>
         </is>
       </c>
       <c r="C25" s="2" t="inlineStr"/>
       <c r="D25" s="2" t="inlineStr"/>
       <c r="E25" s="2" t="inlineStr">
         <is>
-          <t>Cattle raised for sale as breeding animals.</t>
+          <t>Aquaculture: includes peal oysters, edible oysters, abalone, mussels.</t>
         </is>
       </c>
       <c r="F25" s="2" t="inlineStr"/>
@@ -856,14 +856,14 @@
       <c r="A26" s="2" t="n"/>
       <c r="B26" s="2" t="inlineStr">
         <is>
-          <t>chickens meat</t>
+          <t>ostriches</t>
         </is>
       </c>
       <c r="C26" s="2" t="inlineStr"/>
       <c r="D26" s="2" t="inlineStr"/>
       <c r="E26" s="2" t="inlineStr">
         <is>
-          <t>Poultry farms. Production mainly for meat.</t>
+          <t>Poultry farming.</t>
         </is>
       </c>
       <c r="F26" s="2" t="inlineStr"/>
@@ -872,14 +872,14 @@
       <c r="A27" s="2" t="n"/>
       <c r="B27" s="2" t="inlineStr">
         <is>
-          <t>dogs</t>
+          <t>pigs</t>
         </is>
       </c>
       <c r="C27" s="2" t="inlineStr"/>
       <c r="D27" s="2" t="inlineStr"/>
       <c r="E27" s="2" t="inlineStr">
         <is>
-          <t>Includes dog breeding, kennels, or areas used for quarantine of dogs related to import or export.</t>
+          <t>Piggeries.</t>
         </is>
       </c>
       <c r="F27" s="2" t="inlineStr"/>
@@ -888,14 +888,14 @@
       <c r="A28" s="2" t="n"/>
       <c r="B28" s="2" t="inlineStr">
         <is>
-          <t>emus</t>
+          <t>sheep</t>
         </is>
       </c>
       <c r="C28" s="2" t="inlineStr"/>
       <c r="D28" s="2" t="inlineStr"/>
       <c r="E28" s="2" t="inlineStr">
         <is>
-          <t>Poultry farms.</t>
+          <t>Specify meat, dairy, stud or wool where appropriate.</t>
         </is>
       </c>
       <c r="F28" s="2" t="inlineStr"/>
@@ -904,14 +904,14 @@
       <c r="A29" s="2" t="n"/>
       <c r="B29" s="2" t="inlineStr">
         <is>
-          <t>goats dairy</t>
+          <t>sheep dairy</t>
         </is>
       </c>
       <c r="C29" s="2" t="inlineStr"/>
       <c r="D29" s="2" t="inlineStr"/>
       <c r="E29" s="2" t="inlineStr">
         <is>
-          <t>Goats for milk production.</t>
+          <t>Sheep for milk production.</t>
         </is>
       </c>
       <c r="F29" s="2" t="inlineStr"/>
@@ -920,14 +920,14 @@
       <c r="A30" s="2" t="n"/>
       <c r="B30" s="2" t="inlineStr">
         <is>
-          <t>geese</t>
+          <t>sheep meat</t>
         </is>
       </c>
       <c r="C30" s="2" t="inlineStr"/>
       <c r="D30" s="2" t="inlineStr"/>
       <c r="E30" s="2" t="inlineStr">
         <is>
-          <t>Poultry farms.</t>
+          <t>Sheep for meat production.</t>
         </is>
       </c>
       <c r="F30" s="2" t="inlineStr"/>
@@ -936,14 +936,14 @@
       <c r="A31" s="2" t="n"/>
       <c r="B31" s="2" t="inlineStr">
         <is>
-          <t>chickens</t>
+          <t>sheep stud</t>
         </is>
       </c>
       <c r="C31" s="2" t="inlineStr"/>
       <c r="D31" s="2" t="inlineStr"/>
       <c r="E31" s="2" t="inlineStr">
         <is>
-          <t>Poultry farms. Specify whether for eggs or meat where possible.</t>
+          <t>Sheep raised for sale as breeding animals.</t>
         </is>
       </c>
       <c r="F31" s="2" t="inlineStr"/>
@@ -952,14 +952,14 @@
       <c r="A32" s="2" t="n"/>
       <c r="B32" s="2" t="inlineStr">
         <is>
-          <t>ducks</t>
+          <t>sheep wool</t>
         </is>
       </c>
       <c r="C32" s="2" t="inlineStr"/>
       <c r="D32" s="2" t="inlineStr"/>
       <c r="E32" s="2" t="inlineStr">
         <is>
-          <t>Poultry farms.</t>
+          <t>Sheep for fibre production.</t>
         </is>
       </c>
       <c r="F32" s="2" t="inlineStr"/>
@@ -968,14 +968,14 @@
       <c r="A33" s="2" t="n"/>
       <c r="B33" s="2" t="inlineStr">
         <is>
-          <t>goats meat</t>
+          <t>turkeys</t>
         </is>
       </c>
       <c r="C33" s="2" t="inlineStr"/>
       <c r="D33" s="2" t="inlineStr"/>
       <c r="E33" s="2" t="inlineStr">
         <is>
-          <t>Goats for meat production.</t>
+          <t>Poultry farms.</t>
         </is>
       </c>
       <c r="F33" s="2" t="inlineStr"/>
@@ -988,35 +988,35 @@
       </c>
       <c r="B34" s="2" t="inlineStr">
         <is>
-          <t>buckwheat</t>
+          <t>barley</t>
         </is>
       </c>
       <c r="C34" s="2" t="inlineStr"/>
       <c r="D34" s="2" t="inlineStr"/>
-      <c r="E34" s="2" t="inlineStr">
-        <is>
-          <t>Buckwheat is a pseudocereal related to rhubarb. As it is grown as a grain it is considered part of cereals.</t>
-        </is>
-      </c>
+      <c r="E34" s="2" t="inlineStr"/>
       <c r="F34" s="2" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n"/>
       <c r="B35" s="2" t="inlineStr">
         <is>
-          <t>rice</t>
+          <t>buckwheat</t>
         </is>
       </c>
       <c r="C35" s="2" t="inlineStr"/>
       <c r="D35" s="2" t="inlineStr"/>
-      <c r="E35" s="2" t="inlineStr"/>
+      <c r="E35" s="2" t="inlineStr">
+        <is>
+          <t>Buckwheat is a pseudocereal related to rhubarb. As it is grown as a grain it is considered part of cereals.</t>
+        </is>
+      </c>
       <c r="F35" s="2" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n"/>
       <c r="B36" s="2" t="inlineStr">
         <is>
-          <t>triticale</t>
+          <t>canary_seed</t>
         </is>
       </c>
       <c r="C36" s="2" t="inlineStr"/>
@@ -1028,7 +1028,7 @@
       <c r="A37" s="2" t="n"/>
       <c r="B37" s="2" t="inlineStr">
         <is>
-          <t>oats</t>
+          <t>maize</t>
         </is>
       </c>
       <c r="C37" s="2" t="inlineStr"/>
@@ -1052,7 +1052,7 @@
       <c r="A39" s="2" t="n"/>
       <c r="B39" s="2" t="inlineStr">
         <is>
-          <t>barley</t>
+          <t>oats</t>
         </is>
       </c>
       <c r="C39" s="2" t="inlineStr"/>
@@ -1080,23 +1080,19 @@
       <c r="A41" s="2" t="n"/>
       <c r="B41" s="2" t="inlineStr">
         <is>
-          <t>sorghum grain</t>
+          <t>rice</t>
         </is>
       </c>
       <c r="C41" s="2" t="inlineStr"/>
       <c r="D41" s="2" t="inlineStr"/>
-      <c r="E41" s="2" t="inlineStr">
-        <is>
-          <t>Sorghum grown for grain. Excludes forage sorghum.</t>
-        </is>
-      </c>
+      <c r="E41" s="2" t="inlineStr"/>
       <c r="F41" s="2" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n"/>
       <c r="B42" s="2" t="inlineStr">
         <is>
-          <t>wheat</t>
+          <t>rye cereal</t>
         </is>
       </c>
       <c r="C42" s="2" t="inlineStr"/>
@@ -1108,19 +1104,23 @@
       <c r="A43" s="2" t="n"/>
       <c r="B43" s="2" t="inlineStr">
         <is>
-          <t>maize</t>
+          <t>sorghum grain</t>
         </is>
       </c>
       <c r="C43" s="2" t="inlineStr"/>
       <c r="D43" s="2" t="inlineStr"/>
-      <c r="E43" s="2" t="inlineStr"/>
+      <c r="E43" s="2" t="inlineStr">
+        <is>
+          <t>Sorghum grown for grain. Excludes forage sorghum.</t>
+        </is>
+      </c>
       <c r="F43" s="2" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n"/>
       <c r="B44" s="2" t="inlineStr">
         <is>
-          <t>canary_seed</t>
+          <t>triticale</t>
         </is>
       </c>
       <c r="C44" s="2" t="inlineStr"/>
@@ -1132,7 +1132,7 @@
       <c r="A45" s="2" t="n"/>
       <c r="B45" s="2" t="inlineStr">
         <is>
-          <t>rye cereal</t>
+          <t>wheat</t>
         </is>
       </c>
       <c r="C45" s="2" t="inlineStr"/>
@@ -1148,7 +1148,7 @@
       </c>
       <c r="B46" s="2" t="inlineStr">
         <is>
-          <t>essential oil crops</t>
+          <t>aloe vera</t>
         </is>
       </c>
       <c r="C46" s="2" t="inlineStr"/>
@@ -1160,7 +1160,7 @@
       <c r="A47" s="2" t="n"/>
       <c r="B47" s="2" t="inlineStr">
         <is>
-          <t>tea</t>
+          <t>cocoa</t>
         </is>
       </c>
       <c r="C47" s="2" t="inlineStr"/>
@@ -1172,7 +1172,7 @@
       <c r="A48" s="2" t="n"/>
       <c r="B48" s="2" t="inlineStr">
         <is>
-          <t>jute</t>
+          <t>coffee</t>
         </is>
       </c>
       <c r="C48" s="2" t="inlineStr"/>
@@ -1184,7 +1184,7 @@
       <c r="A49" s="2" t="n"/>
       <c r="B49" s="2" t="inlineStr">
         <is>
-          <t>cocoa</t>
+          <t>cotton</t>
         </is>
       </c>
       <c r="C49" s="2" t="inlineStr"/>
@@ -1196,7 +1196,7 @@
       <c r="A50" s="2" t="n"/>
       <c r="B50" s="2" t="inlineStr">
         <is>
-          <t>wasabi</t>
+          <t>cotton seed</t>
         </is>
       </c>
       <c r="C50" s="2" t="inlineStr"/>
@@ -1208,7 +1208,7 @@
       <c r="A51" s="2" t="n"/>
       <c r="B51" s="2" t="inlineStr">
         <is>
-          <t>aloe vera</t>
+          <t>essential oil crops</t>
         </is>
       </c>
       <c r="C51" s="2" t="inlineStr"/>
@@ -1220,7 +1220,7 @@
       <c r="A52" s="2" t="n"/>
       <c r="B52" s="2" t="inlineStr">
         <is>
-          <t>hops</t>
+          <t>ginger</t>
         </is>
       </c>
       <c r="C52" s="2" t="inlineStr"/>
@@ -1232,7 +1232,7 @@
       <c r="A53" s="2" t="n"/>
       <c r="B53" s="2" t="inlineStr">
         <is>
-          <t>sugar cane</t>
+          <t>hops</t>
         </is>
       </c>
       <c r="C53" s="2" t="inlineStr"/>
@@ -1244,7 +1244,7 @@
       <c r="A54" s="2" t="n"/>
       <c r="B54" s="2" t="inlineStr">
         <is>
-          <t>coffee</t>
+          <t>horseradish</t>
         </is>
       </c>
       <c r="C54" s="2" t="inlineStr"/>
@@ -1256,7 +1256,7 @@
       <c r="A55" s="2" t="n"/>
       <c r="B55" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">poppies </t>
+          <t>jute</t>
         </is>
       </c>
       <c r="C55" s="2" t="inlineStr"/>
@@ -1268,7 +1268,7 @@
       <c r="A56" s="2" t="n"/>
       <c r="B56" s="2" t="inlineStr">
         <is>
-          <t>tobacco</t>
+          <t>oil palms</t>
         </is>
       </c>
       <c r="C56" s="2" t="inlineStr"/>
@@ -1280,7 +1280,7 @@
       <c r="A57" s="2" t="n"/>
       <c r="B57" s="2" t="inlineStr">
         <is>
-          <t>horseradish</t>
+          <t>pepper</t>
         </is>
       </c>
       <c r="C57" s="2" t="inlineStr"/>
@@ -1292,7 +1292,7 @@
       <c r="A58" s="2" t="n"/>
       <c r="B58" s="2" t="inlineStr">
         <is>
-          <t>cotton seed</t>
+          <t>pharmaceutical and cosmetic plants</t>
         </is>
       </c>
       <c r="C58" s="2" t="inlineStr"/>
@@ -1304,7 +1304,7 @@
       <c r="A59" s="2" t="n"/>
       <c r="B59" s="2" t="inlineStr">
         <is>
-          <t>pyrethrum</t>
+          <t xml:space="preserve">poppies </t>
         </is>
       </c>
       <c r="C59" s="2" t="inlineStr"/>
@@ -1316,7 +1316,7 @@
       <c r="A60" s="2" t="n"/>
       <c r="B60" s="2" t="inlineStr">
         <is>
-          <t>ginger</t>
+          <t>pyrethrum</t>
         </is>
       </c>
       <c r="C60" s="2" t="inlineStr"/>
@@ -1328,7 +1328,7 @@
       <c r="A61" s="2" t="n"/>
       <c r="B61" s="2" t="inlineStr">
         <is>
-          <t>pharmaceutical and cosmetic plants</t>
+          <t>sugar cane</t>
         </is>
       </c>
       <c r="C61" s="2" t="inlineStr"/>
@@ -1340,7 +1340,7 @@
       <c r="A62" s="2" t="n"/>
       <c r="B62" s="2" t="inlineStr">
         <is>
-          <t>oil palms</t>
+          <t>tea</t>
         </is>
       </c>
       <c r="C62" s="2" t="inlineStr"/>
@@ -1352,7 +1352,7 @@
       <c r="A63" s="2" t="n"/>
       <c r="B63" s="2" t="inlineStr">
         <is>
-          <t>pepper</t>
+          <t>tobacco</t>
         </is>
       </c>
       <c r="C63" s="2" t="inlineStr"/>
@@ -1364,7 +1364,7 @@
       <c r="A64" s="2" t="n"/>
       <c r="B64" s="2" t="inlineStr">
         <is>
-          <t>cotton</t>
+          <t>wasabi</t>
         </is>
       </c>
       <c r="C64" s="2" t="inlineStr"/>
@@ -1380,7 +1380,7 @@
       </c>
       <c r="B65" s="2" t="inlineStr">
         <is>
-          <t>bulbs</t>
+          <t>australian native flowers</t>
         </is>
       </c>
       <c r="C65" s="2" t="inlineStr"/>
@@ -1392,7 +1392,7 @@
       <c r="A66" s="2" t="n"/>
       <c r="B66" s="2" t="inlineStr">
         <is>
-          <t>proteas</t>
+          <t>bulbs</t>
         </is>
       </c>
       <c r="C66" s="2" t="inlineStr"/>
@@ -1404,7 +1404,7 @@
       <c r="A67" s="2" t="n"/>
       <c r="B67" s="2" t="inlineStr">
         <is>
-          <t>carnations</t>
+          <t>calendula</t>
         </is>
       </c>
       <c r="C67" s="2" t="inlineStr"/>
@@ -1416,7 +1416,7 @@
       <c r="A68" s="2" t="n"/>
       <c r="B68" s="2" t="inlineStr">
         <is>
-          <t>lavender</t>
+          <t>carnations</t>
         </is>
       </c>
       <c r="C68" s="2" t="inlineStr"/>
@@ -1428,7 +1428,7 @@
       <c r="A69" s="2" t="n"/>
       <c r="B69" s="2" t="inlineStr">
         <is>
-          <t>lilies</t>
+          <t>chrysanthemums</t>
         </is>
       </c>
       <c r="C69" s="2" t="inlineStr"/>
@@ -1440,7 +1440,7 @@
       <c r="A70" s="2" t="n"/>
       <c r="B70" s="2" t="inlineStr">
         <is>
-          <t>roses</t>
+          <t>daffodils</t>
         </is>
       </c>
       <c r="C70" s="2" t="inlineStr"/>
@@ -1452,7 +1452,7 @@
       <c r="A71" s="2" t="n"/>
       <c r="B71" s="2" t="inlineStr">
         <is>
-          <t>tropical flowers</t>
+          <t>flowers and foliage</t>
         </is>
       </c>
       <c r="C71" s="2" t="inlineStr"/>
@@ -1464,7 +1464,7 @@
       <c r="A72" s="2" t="n"/>
       <c r="B72" s="2" t="inlineStr">
         <is>
-          <t>chrysanthemums</t>
+          <t>gerberas</t>
         </is>
       </c>
       <c r="C72" s="2" t="inlineStr"/>
@@ -1476,7 +1476,7 @@
       <c r="A73" s="2" t="n"/>
       <c r="B73" s="2" t="inlineStr">
         <is>
-          <t>calendula</t>
+          <t>lavender</t>
         </is>
       </c>
       <c r="C73" s="2" t="inlineStr"/>
@@ -1488,7 +1488,7 @@
       <c r="A74" s="2" t="n"/>
       <c r="B74" s="2" t="inlineStr">
         <is>
-          <t>tulips</t>
+          <t>lilies</t>
         </is>
       </c>
       <c r="C74" s="2" t="inlineStr"/>
@@ -1500,7 +1500,7 @@
       <c r="A75" s="2" t="n"/>
       <c r="B75" s="2" t="inlineStr">
         <is>
-          <t>daffodils</t>
+          <t>orchids</t>
         </is>
       </c>
       <c r="C75" s="2" t="inlineStr"/>
@@ -1512,7 +1512,7 @@
       <c r="A76" s="2" t="n"/>
       <c r="B76" s="2" t="inlineStr">
         <is>
-          <t>gerberas</t>
+          <t>proteas</t>
         </is>
       </c>
       <c r="C76" s="2" t="inlineStr"/>
@@ -1524,7 +1524,7 @@
       <c r="A77" s="2" t="n"/>
       <c r="B77" s="2" t="inlineStr">
         <is>
-          <t>australian native flowers</t>
+          <t>roses</t>
         </is>
       </c>
       <c r="C77" s="2" t="inlineStr"/>
@@ -1536,7 +1536,7 @@
       <c r="A78" s="2" t="n"/>
       <c r="B78" s="2" t="inlineStr">
         <is>
-          <t>flowers and foliage</t>
+          <t>tropical flowers</t>
         </is>
       </c>
       <c r="C78" s="2" t="inlineStr"/>
@@ -1548,7 +1548,7 @@
       <c r="A79" s="2" t="n"/>
       <c r="B79" s="2" t="inlineStr">
         <is>
-          <t>orchids</t>
+          <t>tulips</t>
         </is>
       </c>
       <c r="C79" s="2" t="inlineStr"/>
@@ -1564,7 +1564,7 @@
       </c>
       <c r="B80" s="2" t="inlineStr">
         <is>
-          <t>christmas trees</t>
+          <t>bamboo</t>
         </is>
       </c>
       <c r="C80" s="2" t="inlineStr"/>
@@ -1576,11 +1576,15 @@
       <c r="A81" s="2" t="n"/>
       <c r="B81" s="2" t="inlineStr">
         <is>
-          <t>sandalwood</t>
+          <t>carbon forest permanent</t>
         </is>
       </c>
       <c r="C81" s="2" t="inlineStr"/>
-      <c r="D81" s="2" t="inlineStr"/>
+      <c r="D81" s="2" t="inlineStr">
+        <is>
+          <t>Permanent carbon forestry under the ETS. These are post-1989 forests that will not be clear-felled. They are expected to remain in permanent forestry for at least 50 years. Before 1 January 2023, the ETS didn't distinguish between standard and permanent forestry. Post-1989 forest land that entered the ETS before 1 January 2023 is standard forestry, unless an application has been accepted to change it to permanent forestry.</t>
+        </is>
+      </c>
       <c r="E81" s="2" t="inlineStr"/>
       <c r="F81" s="2" t="inlineStr"/>
     </row>
@@ -1588,11 +1592,15 @@
       <c r="A82" s="2" t="n"/>
       <c r="B82" s="2" t="inlineStr">
         <is>
-          <t>bamboo</t>
+          <t>carbon forest standard</t>
         </is>
       </c>
       <c r="C82" s="2" t="inlineStr"/>
-      <c r="D82" s="2" t="inlineStr"/>
+      <c r="D82" s="2" t="inlineStr">
+        <is>
+          <t>Standard carbon foresty under the ETS. Standard forestry refers to post-1989 forests under the ETS that are expected to be regularly harvested and replanted, such as commercial plantation forests. Other commodities (such as sawlog) are compatible.</t>
+        </is>
+      </c>
       <c r="E82" s="2" t="inlineStr"/>
       <c r="F82" s="2" t="inlineStr"/>
     </row>
@@ -1600,7 +1608,7 @@
       <c r="A83" s="2" t="n"/>
       <c r="B83" s="2" t="inlineStr">
         <is>
-          <t>eucalyptus oil</t>
+          <t>christmas trees</t>
         </is>
       </c>
       <c r="C83" s="2" t="inlineStr"/>
@@ -1612,7 +1620,7 @@
       <c r="A84" s="2" t="n"/>
       <c r="B84" s="2" t="inlineStr">
         <is>
-          <t>tea tree</t>
+          <t>eucalyptus oil</t>
         </is>
       </c>
       <c r="C84" s="2" t="inlineStr"/>
@@ -1648,7 +1656,7 @@
       <c r="A87" s="2" t="n"/>
       <c r="B87" s="2" t="inlineStr">
         <is>
-          <t>sawlogs</t>
+          <t>sandalwood</t>
         </is>
       </c>
       <c r="C87" s="2" t="inlineStr"/>
@@ -1660,15 +1668,11 @@
       <c r="A88" s="2" t="n"/>
       <c r="B88" s="2" t="inlineStr">
         <is>
-          <t>carbon forest permanent</t>
+          <t>sawlogs</t>
         </is>
       </c>
       <c r="C88" s="2" t="inlineStr"/>
-      <c r="D88" s="2" t="inlineStr">
-        <is>
-          <t>Permanent carbon forestry under the ETS. These are post-1989 forests that will not be clear-felled. They are expected to remain in permanent forestry for at least 50 years. Before 1 January 2023, the ETS didn't distinguish between standard and permanent forestry. Post-1989 forest land that entered the ETS before 1 January 2023 is standard forestry, unless an application has been accepted to change it to permanent forestry.</t>
-        </is>
-      </c>
+      <c r="D88" s="2" t="inlineStr"/>
       <c r="E88" s="2" t="inlineStr"/>
       <c r="F88" s="2" t="inlineStr"/>
     </row>
@@ -1676,15 +1680,11 @@
       <c r="A89" s="2" t="n"/>
       <c r="B89" s="2" t="inlineStr">
         <is>
-          <t>carbon forest standard</t>
+          <t>tea tree</t>
         </is>
       </c>
       <c r="C89" s="2" t="inlineStr"/>
-      <c r="D89" s="2" t="inlineStr">
-        <is>
-          <t>Standard carbon foresty under the ETS. Standard forestry refers to post-1989 forests under the ETS that are expected to be regularly harvested and replanted, such as commercial plantation forests. Other commodities (such as sawlog) are compatible.</t>
-        </is>
-      </c>
+      <c r="D89" s="2" t="inlineStr"/>
       <c r="E89" s="2" t="inlineStr"/>
       <c r="F89" s="2" t="inlineStr"/>
     </row>
@@ -1696,7 +1696,7 @@
       </c>
       <c r="B90" s="2" t="inlineStr">
         <is>
-          <t>cranberries</t>
+          <t>apples</t>
         </is>
       </c>
       <c r="C90" s="2" t="inlineStr"/>
@@ -1708,7 +1708,7 @@
       <c r="A91" s="2" t="n"/>
       <c r="B91" s="2" t="inlineStr">
         <is>
-          <t>pineapples</t>
+          <t>apricots</t>
         </is>
       </c>
       <c r="C91" s="2" t="inlineStr"/>
@@ -1720,7 +1720,7 @@
       <c r="A92" s="2" t="n"/>
       <c r="B92" s="2" t="inlineStr">
         <is>
-          <t>persimmons</t>
+          <t>avocados</t>
         </is>
       </c>
       <c r="C92" s="2" t="inlineStr"/>
@@ -1732,7 +1732,7 @@
       <c r="A93" s="2" t="n"/>
       <c r="B93" s="2" t="inlineStr">
         <is>
-          <t>blackcurrants</t>
+          <t>babacos</t>
         </is>
       </c>
       <c r="C93" s="2" t="inlineStr"/>
@@ -1744,7 +1744,7 @@
       <c r="A94" s="2" t="n"/>
       <c r="B94" s="2" t="inlineStr">
         <is>
-          <t>babacos</t>
+          <t>bananas</t>
         </is>
       </c>
       <c r="C94" s="2" t="inlineStr"/>
@@ -1756,7 +1756,7 @@
       <c r="A95" s="2" t="n"/>
       <c r="B95" s="2" t="inlineStr">
         <is>
-          <t>loquats</t>
+          <t>blackberries</t>
         </is>
       </c>
       <c r="C95" s="2" t="inlineStr"/>
@@ -1768,7 +1768,7 @@
       <c r="A96" s="2" t="n"/>
       <c r="B96" s="2" t="inlineStr">
         <is>
-          <t>boysenberries</t>
+          <t>blackcurrants</t>
         </is>
       </c>
       <c r="C96" s="2" t="inlineStr"/>
@@ -1780,7 +1780,7 @@
       <c r="A97" s="2" t="n"/>
       <c r="B97" s="2" t="inlineStr">
         <is>
-          <t>mulberries</t>
+          <t>blueberries</t>
         </is>
       </c>
       <c r="C97" s="2" t="inlineStr"/>
@@ -1792,7 +1792,7 @@
       <c r="A98" s="2" t="n"/>
       <c r="B98" s="2" t="inlineStr">
         <is>
-          <t>apples</t>
+          <t>boysenberries</t>
         </is>
       </c>
       <c r="C98" s="2" t="inlineStr"/>
@@ -1804,7 +1804,7 @@
       <c r="A99" s="2" t="n"/>
       <c r="B99" s="2" t="inlineStr">
         <is>
-          <t>mangosteen</t>
+          <t>carambolas</t>
         </is>
       </c>
       <c r="C99" s="2" t="inlineStr"/>
@@ -1816,7 +1816,7 @@
       <c r="A100" s="2" t="n"/>
       <c r="B100" s="2" t="inlineStr">
         <is>
-          <t>peacharines</t>
+          <t>cherries</t>
         </is>
       </c>
       <c r="C100" s="2" t="inlineStr"/>
@@ -1828,7 +1828,7 @@
       <c r="A101" s="2" t="n"/>
       <c r="B101" s="2" t="inlineStr">
         <is>
-          <t>coconut</t>
+          <t>chokos</t>
         </is>
       </c>
       <c r="C101" s="2" t="inlineStr"/>
@@ -1840,7 +1840,7 @@
       <c r="A102" s="2" t="n"/>
       <c r="B102" s="2" t="inlineStr">
         <is>
-          <t>chokos</t>
+          <t>coconut</t>
         </is>
       </c>
       <c r="C102" s="2" t="inlineStr"/>
@@ -1852,7 +1852,7 @@
       <c r="A103" s="2" t="n"/>
       <c r="B103" s="2" t="inlineStr">
         <is>
-          <t>lychees</t>
+          <t>cranberries</t>
         </is>
       </c>
       <c r="C103" s="2" t="inlineStr"/>
@@ -1864,7 +1864,7 @@
       <c r="A104" s="2" t="n"/>
       <c r="B104" s="2" t="inlineStr">
         <is>
-          <t>grapes</t>
+          <t>custard apples</t>
         </is>
       </c>
       <c r="C104" s="2" t="inlineStr"/>
@@ -1876,7 +1876,7 @@
       <c r="A105" s="2" t="n"/>
       <c r="B105" s="2" t="inlineStr">
         <is>
-          <t>apricots</t>
+          <t>dates</t>
         </is>
       </c>
       <c r="C105" s="2" t="inlineStr"/>
@@ -1888,7 +1888,7 @@
       <c r="A106" s="2" t="n"/>
       <c r="B106" s="2" t="inlineStr">
         <is>
-          <t>mangoes</t>
+          <t>dragon fruit</t>
         </is>
       </c>
       <c r="C106" s="2" t="inlineStr"/>
@@ -1900,7 +1900,7 @@
       <c r="A107" s="2" t="n"/>
       <c r="B107" s="2" t="inlineStr">
         <is>
-          <t>olives</t>
+          <t>feijoa</t>
         </is>
       </c>
       <c r="C107" s="2" t="inlineStr"/>
@@ -1912,7 +1912,7 @@
       <c r="A108" s="2" t="n"/>
       <c r="B108" s="2" t="inlineStr">
         <is>
-          <t>plums</t>
+          <t>figs</t>
         </is>
       </c>
       <c r="C108" s="2" t="inlineStr"/>
@@ -1924,7 +1924,7 @@
       <c r="A109" s="2" t="n"/>
       <c r="B109" s="2" t="inlineStr">
         <is>
-          <t>guavas</t>
+          <t>gooseberries</t>
         </is>
       </c>
       <c r="C109" s="2" t="inlineStr"/>
@@ -1936,7 +1936,7 @@
       <c r="A110" s="2" t="n"/>
       <c r="B110" s="2" t="inlineStr">
         <is>
-          <t>grapes wine</t>
+          <t>grapefruit</t>
         </is>
       </c>
       <c r="C110" s="2" t="inlineStr"/>
@@ -1948,7 +1948,7 @@
       <c r="A111" s="2" t="n"/>
       <c r="B111" s="2" t="inlineStr">
         <is>
-          <t>oranges</t>
+          <t>grapes</t>
         </is>
       </c>
       <c r="C111" s="2" t="inlineStr"/>
@@ -1960,7 +1960,7 @@
       <c r="A112" s="2" t="n"/>
       <c r="B112" s="2" t="inlineStr">
         <is>
-          <t>pawpaws</t>
+          <t>grapes dried</t>
         </is>
       </c>
       <c r="C112" s="2" t="inlineStr"/>
@@ -1972,7 +1972,7 @@
       <c r="A113" s="2" t="n"/>
       <c r="B113" s="2" t="inlineStr">
         <is>
-          <t>quinces</t>
+          <t>grapes table</t>
         </is>
       </c>
       <c r="C113" s="2" t="inlineStr"/>
@@ -1984,7 +1984,7 @@
       <c r="A114" s="2" t="n"/>
       <c r="B114" s="2" t="inlineStr">
         <is>
-          <t>mandarins</t>
+          <t>grapes wine</t>
         </is>
       </c>
       <c r="C114" s="2" t="inlineStr"/>
@@ -1996,7 +1996,7 @@
       <c r="A115" s="2" t="n"/>
       <c r="B115" s="2" t="inlineStr">
         <is>
-          <t>redcurrants</t>
+          <t>guavas</t>
         </is>
       </c>
       <c r="C115" s="2" t="inlineStr"/>
@@ -2008,7 +2008,7 @@
       <c r="A116" s="2" t="n"/>
       <c r="B116" s="2" t="inlineStr">
         <is>
-          <t>tangelos</t>
+          <t>jackfruit</t>
         </is>
       </c>
       <c r="C116" s="2" t="inlineStr"/>
@@ -2020,7 +2020,7 @@
       <c r="A117" s="2" t="n"/>
       <c r="B117" s="2" t="inlineStr">
         <is>
-          <t>grapes table</t>
+          <t>kiwifruit</t>
         </is>
       </c>
       <c r="C117" s="2" t="inlineStr"/>
@@ -2032,7 +2032,7 @@
       <c r="A118" s="2" t="n"/>
       <c r="B118" s="2" t="inlineStr">
         <is>
-          <t>pomegranate</t>
+          <t>kumquat</t>
         </is>
       </c>
       <c r="C118" s="2" t="inlineStr"/>
@@ -2044,7 +2044,7 @@
       <c r="A119" s="2" t="n"/>
       <c r="B119" s="2" t="inlineStr">
         <is>
-          <t>passionfruit</t>
+          <t>lemons</t>
         </is>
       </c>
       <c r="C119" s="2" t="inlineStr"/>
@@ -2056,7 +2056,7 @@
       <c r="A120" s="2" t="n"/>
       <c r="B120" s="2" t="inlineStr">
         <is>
-          <t>kiwifruit</t>
+          <t>limes</t>
         </is>
       </c>
       <c r="C120" s="2" t="inlineStr"/>
@@ -2068,7 +2068,7 @@
       <c r="A121" s="2" t="n"/>
       <c r="B121" s="2" t="inlineStr">
         <is>
-          <t>gooseberries</t>
+          <t>loganberries</t>
         </is>
       </c>
       <c r="C121" s="2" t="inlineStr"/>
@@ -2080,7 +2080,7 @@
       <c r="A122" s="2" t="n"/>
       <c r="B122" s="2" t="inlineStr">
         <is>
-          <t>peaches</t>
+          <t>longans</t>
         </is>
       </c>
       <c r="C122" s="2" t="inlineStr"/>
@@ -2092,7 +2092,7 @@
       <c r="A123" s="2" t="n"/>
       <c r="B123" s="2" t="inlineStr">
         <is>
-          <t>feijoa</t>
+          <t>loquats</t>
         </is>
       </c>
       <c r="C123" s="2" t="inlineStr"/>
@@ -2104,7 +2104,7 @@
       <c r="A124" s="2" t="n"/>
       <c r="B124" s="2" t="inlineStr">
         <is>
-          <t>kumquat</t>
+          <t>lychees</t>
         </is>
       </c>
       <c r="C124" s="2" t="inlineStr"/>
@@ -2116,7 +2116,7 @@
       <c r="A125" s="2" t="n"/>
       <c r="B125" s="2" t="inlineStr">
         <is>
-          <t>limes</t>
+          <t>mandarins</t>
         </is>
       </c>
       <c r="C125" s="2" t="inlineStr"/>
@@ -2128,7 +2128,7 @@
       <c r="A126" s="2" t="n"/>
       <c r="B126" s="2" t="inlineStr">
         <is>
-          <t>nectarines</t>
+          <t>mangoes</t>
         </is>
       </c>
       <c r="C126" s="2" t="inlineStr"/>
@@ -2140,7 +2140,7 @@
       <c r="A127" s="2" t="n"/>
       <c r="B127" s="2" t="inlineStr">
         <is>
-          <t>tamarillo</t>
+          <t>mangosteen</t>
         </is>
       </c>
       <c r="C127" s="2" t="inlineStr"/>
@@ -2152,7 +2152,7 @@
       <c r="A128" s="2" t="n"/>
       <c r="B128" s="2" t="inlineStr">
         <is>
-          <t>bananas</t>
+          <t>melons</t>
         </is>
       </c>
       <c r="C128" s="2" t="inlineStr"/>
@@ -2164,7 +2164,7 @@
       <c r="A129" s="2" t="n"/>
       <c r="B129" s="2" t="inlineStr">
         <is>
-          <t>custard apples</t>
+          <t>mulberries</t>
         </is>
       </c>
       <c r="C129" s="2" t="inlineStr"/>
@@ -2176,7 +2176,7 @@
       <c r="A130" s="2" t="n"/>
       <c r="B130" s="2" t="inlineStr">
         <is>
-          <t>cherries</t>
+          <t>nectarines</t>
         </is>
       </c>
       <c r="C130" s="2" t="inlineStr"/>
@@ -2188,7 +2188,7 @@
       <c r="A131" s="2" t="n"/>
       <c r="B131" s="2" t="inlineStr">
         <is>
-          <t>loganberries</t>
+          <t>olives</t>
         </is>
       </c>
       <c r="C131" s="2" t="inlineStr"/>
@@ -2200,7 +2200,7 @@
       <c r="A132" s="2" t="n"/>
       <c r="B132" s="2" t="inlineStr">
         <is>
-          <t>pears nashi</t>
+          <t>oranges</t>
         </is>
       </c>
       <c r="C132" s="2" t="inlineStr"/>
@@ -2212,7 +2212,7 @@
       <c r="A133" s="2" t="n"/>
       <c r="B133" s="2" t="inlineStr">
         <is>
-          <t>pears</t>
+          <t>passionfruit</t>
         </is>
       </c>
       <c r="C133" s="2" t="inlineStr"/>
@@ -2224,7 +2224,7 @@
       <c r="A134" s="2" t="n"/>
       <c r="B134" s="2" t="inlineStr">
         <is>
-          <t>rosella</t>
+          <t>pawpaws</t>
         </is>
       </c>
       <c r="C134" s="2" t="inlineStr"/>
@@ -2236,7 +2236,7 @@
       <c r="A135" s="2" t="n"/>
       <c r="B135" s="2" t="inlineStr">
         <is>
-          <t>carambolas</t>
+          <t>peacharines</t>
         </is>
       </c>
       <c r="C135" s="2" t="inlineStr"/>
@@ -2248,7 +2248,7 @@
       <c r="A136" s="2" t="n"/>
       <c r="B136" s="2" t="inlineStr">
         <is>
-          <t>lemons</t>
+          <t>peaches</t>
         </is>
       </c>
       <c r="C136" s="2" t="inlineStr"/>
@@ -2260,7 +2260,7 @@
       <c r="A137" s="2" t="n"/>
       <c r="B137" s="2" t="inlineStr">
         <is>
-          <t>melons</t>
+          <t>pears</t>
         </is>
       </c>
       <c r="C137" s="2" t="inlineStr"/>
@@ -2272,7 +2272,7 @@
       <c r="A138" s="2" t="n"/>
       <c r="B138" s="2" t="inlineStr">
         <is>
-          <t>dates</t>
+          <t>pears nashi</t>
         </is>
       </c>
       <c r="C138" s="2" t="inlineStr"/>
@@ -2296,7 +2296,7 @@
       <c r="A140" s="2" t="n"/>
       <c r="B140" s="2" t="inlineStr">
         <is>
-          <t>watermelons</t>
+          <t>persimmons</t>
         </is>
       </c>
       <c r="C140" s="2" t="inlineStr"/>
@@ -2308,7 +2308,7 @@
       <c r="A141" s="2" t="n"/>
       <c r="B141" s="2" t="inlineStr">
         <is>
-          <t>jackfruit</t>
+          <t>pineapples</t>
         </is>
       </c>
       <c r="C141" s="2" t="inlineStr"/>
@@ -2320,7 +2320,7 @@
       <c r="A142" s="2" t="n"/>
       <c r="B142" s="2" t="inlineStr">
         <is>
-          <t>blackberries</t>
+          <t>plums</t>
         </is>
       </c>
       <c r="C142" s="2" t="inlineStr"/>
@@ -2332,7 +2332,7 @@
       <c r="A143" s="2" t="n"/>
       <c r="B143" s="2" t="inlineStr">
         <is>
-          <t>longans</t>
+          <t>pomegranate</t>
         </is>
       </c>
       <c r="C143" s="2" t="inlineStr"/>
@@ -2344,7 +2344,7 @@
       <c r="A144" s="2" t="n"/>
       <c r="B144" s="2" t="inlineStr">
         <is>
-          <t>raspberries</t>
+          <t>quinces</t>
         </is>
       </c>
       <c r="C144" s="2" t="inlineStr"/>
@@ -2356,7 +2356,7 @@
       <c r="A145" s="2" t="n"/>
       <c r="B145" s="2" t="inlineStr">
         <is>
-          <t>blueberries</t>
+          <t>rambutans</t>
         </is>
       </c>
       <c r="C145" s="2" t="inlineStr"/>
@@ -2368,7 +2368,7 @@
       <c r="A146" s="2" t="n"/>
       <c r="B146" s="2" t="inlineStr">
         <is>
-          <t>dragon fruit</t>
+          <t>raspberries</t>
         </is>
       </c>
       <c r="C146" s="2" t="inlineStr"/>
@@ -2380,7 +2380,7 @@
       <c r="A147" s="2" t="n"/>
       <c r="B147" s="2" t="inlineStr">
         <is>
-          <t>grapefruit</t>
+          <t>redcurrants</t>
         </is>
       </c>
       <c r="C147" s="2" t="inlineStr"/>
@@ -2392,7 +2392,7 @@
       <c r="A148" s="2" t="n"/>
       <c r="B148" s="2" t="inlineStr">
         <is>
-          <t>rambutans</t>
+          <t>rosella</t>
         </is>
       </c>
       <c r="C148" s="2" t="inlineStr"/>
@@ -2404,7 +2404,7 @@
       <c r="A149" s="2" t="n"/>
       <c r="B149" s="2" t="inlineStr">
         <is>
-          <t>avocados</t>
+          <t>strawberries</t>
         </is>
       </c>
       <c r="C149" s="2" t="inlineStr"/>
@@ -2416,7 +2416,7 @@
       <c r="A150" s="2" t="n"/>
       <c r="B150" s="2" t="inlineStr">
         <is>
-          <t>strawberries</t>
+          <t>tamarillo</t>
         </is>
       </c>
       <c r="C150" s="2" t="inlineStr"/>
@@ -2428,7 +2428,7 @@
       <c r="A151" s="2" t="n"/>
       <c r="B151" s="2" t="inlineStr">
         <is>
-          <t>grapes dried</t>
+          <t>tangelos</t>
         </is>
       </c>
       <c r="C151" s="2" t="inlineStr"/>
@@ -2440,7 +2440,7 @@
       <c r="A152" s="2" t="n"/>
       <c r="B152" s="2" t="inlineStr">
         <is>
-          <t>figs</t>
+          <t>watermelons</t>
         </is>
       </c>
       <c r="C152" s="2" t="inlineStr"/>
@@ -2472,7 +2472,7 @@
       </c>
       <c r="B154" s="2" t="inlineStr">
         <is>
-          <t>aluminium</t>
+          <t>alumina</t>
         </is>
       </c>
       <c r="C154" s="2" t="inlineStr"/>
@@ -2484,7 +2484,7 @@
       <c r="A155" s="2" t="n"/>
       <c r="B155" s="2" t="inlineStr">
         <is>
-          <t>salt</t>
+          <t>aluminium</t>
         </is>
       </c>
       <c r="C155" s="2" t="inlineStr"/>
@@ -2496,7 +2496,7 @@
       <c r="A156" s="2" t="n"/>
       <c r="B156" s="2" t="inlineStr">
         <is>
-          <t>stone</t>
+          <t>bauxite</t>
         </is>
       </c>
       <c r="C156" s="2" t="inlineStr"/>
@@ -2508,7 +2508,7 @@
       <c r="A157" s="2" t="n"/>
       <c r="B157" s="2" t="inlineStr">
         <is>
-          <t>copper</t>
+          <t>coal</t>
         </is>
       </c>
       <c r="C157" s="2" t="inlineStr"/>
@@ -2520,7 +2520,7 @@
       <c r="A158" s="2" t="n"/>
       <c r="B158" s="2" t="inlineStr">
         <is>
-          <t>coal</t>
+          <t xml:space="preserve">coal_black </t>
         </is>
       </c>
       <c r="C158" s="2" t="inlineStr"/>
@@ -2532,7 +2532,7 @@
       <c r="A159" s="2" t="n"/>
       <c r="B159" s="2" t="inlineStr">
         <is>
-          <t>zinc</t>
+          <t xml:space="preserve">coal_brown </t>
         </is>
       </c>
       <c r="C159" s="2" t="inlineStr"/>
@@ -2544,7 +2544,7 @@
       <c r="A160" s="2" t="n"/>
       <c r="B160" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">coal_black </t>
+          <t>copper</t>
         </is>
       </c>
       <c r="C160" s="2" t="inlineStr"/>
@@ -2556,7 +2556,7 @@
       <c r="A161" s="2" t="n"/>
       <c r="B161" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">rare_earths </t>
+          <t xml:space="preserve">diamonds_rough </t>
         </is>
       </c>
       <c r="C161" s="2" t="inlineStr"/>
@@ -2568,7 +2568,7 @@
       <c r="A162" s="2" t="n"/>
       <c r="B162" s="2" t="inlineStr">
         <is>
-          <t>iron_ore</t>
+          <t>gold</t>
         </is>
       </c>
       <c r="C162" s="2" t="inlineStr"/>
@@ -2580,7 +2580,7 @@
       <c r="A163" s="2" t="n"/>
       <c r="B163" s="2" t="inlineStr">
         <is>
-          <t>lead</t>
+          <t>iron_ore</t>
         </is>
       </c>
       <c r="C163" s="2" t="inlineStr"/>
@@ -2592,7 +2592,7 @@
       <c r="A164" s="2" t="n"/>
       <c r="B164" s="2" t="inlineStr">
         <is>
-          <t>zeolite</t>
+          <t>ironsand</t>
         </is>
       </c>
       <c r="C164" s="2" t="inlineStr"/>
@@ -2604,7 +2604,7 @@
       <c r="A165" s="2" t="n"/>
       <c r="B165" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">coal_brown </t>
+          <t>lead</t>
         </is>
       </c>
       <c r="C165" s="2" t="inlineStr"/>
@@ -2616,7 +2616,7 @@
       <c r="A166" s="2" t="n"/>
       <c r="B166" s="2" t="inlineStr">
         <is>
-          <t>uranium</t>
+          <t>metal</t>
         </is>
       </c>
       <c r="C166" s="2" t="inlineStr"/>
@@ -2628,7 +2628,7 @@
       <c r="A167" s="2" t="n"/>
       <c r="B167" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">diamonds_rough </t>
+          <t xml:space="preserve">mineral_sands </t>
         </is>
       </c>
       <c r="C167" s="2" t="inlineStr"/>
@@ -2640,7 +2640,7 @@
       <c r="A168" s="2" t="n"/>
       <c r="B168" s="2" t="inlineStr">
         <is>
-          <t>silica_sand</t>
+          <t>nickel</t>
         </is>
       </c>
       <c r="C168" s="2" t="inlineStr"/>
@@ -2652,7 +2652,7 @@
       <c r="A169" s="2" t="n"/>
       <c r="B169" s="2" t="inlineStr">
         <is>
-          <t>bauxite</t>
+          <t xml:space="preserve">rare_earths </t>
         </is>
       </c>
       <c r="C169" s="2" t="inlineStr"/>
@@ -2664,7 +2664,7 @@
       <c r="A170" s="2" t="n"/>
       <c r="B170" s="2" t="inlineStr">
         <is>
-          <t>gold</t>
+          <t>salt</t>
         </is>
       </c>
       <c r="C170" s="2" t="inlineStr"/>
@@ -2676,7 +2676,7 @@
       <c r="A171" s="2" t="n"/>
       <c r="B171" s="2" t="inlineStr">
         <is>
-          <t>alumina</t>
+          <t>shingle</t>
         </is>
       </c>
       <c r="C171" s="2" t="inlineStr"/>
@@ -2688,7 +2688,7 @@
       <c r="A172" s="2" t="n"/>
       <c r="B172" s="2" t="inlineStr">
         <is>
-          <t>metal</t>
+          <t>silica_sand</t>
         </is>
       </c>
       <c r="C172" s="2" t="inlineStr"/>
@@ -2700,7 +2700,7 @@
       <c r="A173" s="2" t="n"/>
       <c r="B173" s="2" t="inlineStr">
         <is>
-          <t>nickel</t>
+          <t>stone</t>
         </is>
       </c>
       <c r="C173" s="2" t="inlineStr"/>
@@ -2712,7 +2712,7 @@
       <c r="A174" s="2" t="n"/>
       <c r="B174" s="2" t="inlineStr">
         <is>
-          <t>shingle</t>
+          <t>uranium</t>
         </is>
       </c>
       <c r="C174" s="2" t="inlineStr"/>
@@ -2724,7 +2724,7 @@
       <c r="A175" s="2" t="n"/>
       <c r="B175" s="2" t="inlineStr">
         <is>
-          <t>ironsand</t>
+          <t>zeolite</t>
         </is>
       </c>
       <c r="C175" s="2" t="inlineStr"/>
@@ -2736,7 +2736,7 @@
       <c r="A176" s="2" t="n"/>
       <c r="B176" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">mineral_sands </t>
+          <t>zinc</t>
         </is>
       </c>
       <c r="C176" s="2" t="inlineStr"/>
@@ -2752,7 +2752,7 @@
       </c>
       <c r="B177" s="2" t="inlineStr">
         <is>
-          <t>pinenuts</t>
+          <t>almonds</t>
         </is>
       </c>
       <c r="C177" s="2" t="inlineStr"/>
@@ -2764,7 +2764,7 @@
       <c r="A178" s="2" t="n"/>
       <c r="B178" s="2" t="inlineStr">
         <is>
-          <t>pecan nuts</t>
+          <t>brazil nuts</t>
         </is>
       </c>
       <c r="C178" s="2" t="inlineStr"/>
@@ -2776,7 +2776,7 @@
       <c r="A179" s="2" t="n"/>
       <c r="B179" s="2" t="inlineStr">
         <is>
-          <t>walnuts</t>
+          <t>cashews</t>
         </is>
       </c>
       <c r="C179" s="2" t="inlineStr"/>
@@ -2788,7 +2788,7 @@
       <c r="A180" s="2" t="n"/>
       <c r="B180" s="2" t="inlineStr">
         <is>
-          <t>cashews</t>
+          <t>chestnuts</t>
         </is>
       </c>
       <c r="C180" s="2" t="inlineStr"/>
@@ -2800,7 +2800,7 @@
       <c r="A181" s="2" t="n"/>
       <c r="B181" s="2" t="inlineStr">
         <is>
-          <t>macadamias</t>
+          <t>hazelnuts</t>
         </is>
       </c>
       <c r="C181" s="2" t="inlineStr"/>
@@ -2812,7 +2812,7 @@
       <c r="A182" s="2" t="n"/>
       <c r="B182" s="2" t="inlineStr">
         <is>
-          <t>brazil nuts</t>
+          <t>macadamias</t>
         </is>
       </c>
       <c r="C182" s="2" t="inlineStr"/>
@@ -2824,7 +2824,7 @@
       <c r="A183" s="2" t="n"/>
       <c r="B183" s="2" t="inlineStr">
         <is>
-          <t>almonds</t>
+          <t>pecan nuts</t>
         </is>
       </c>
       <c r="C183" s="2" t="inlineStr"/>
@@ -2836,7 +2836,7 @@
       <c r="A184" s="2" t="n"/>
       <c r="B184" s="2" t="inlineStr">
         <is>
-          <t>pistachios</t>
+          <t>pinenuts</t>
         </is>
       </c>
       <c r="C184" s="2" t="inlineStr"/>
@@ -2848,7 +2848,7 @@
       <c r="A185" s="2" t="n"/>
       <c r="B185" s="2" t="inlineStr">
         <is>
-          <t>hazelnuts</t>
+          <t>pistachios</t>
         </is>
       </c>
       <c r="C185" s="2" t="inlineStr"/>
@@ -2860,7 +2860,7 @@
       <c r="A186" s="2" t="n"/>
       <c r="B186" s="2" t="inlineStr">
         <is>
-          <t>chestnuts</t>
+          <t>walnuts</t>
         </is>
       </c>
       <c r="C186" s="2" t="inlineStr"/>
@@ -2888,7 +2888,7 @@
       <c r="A188" s="2" t="n"/>
       <c r="B188" s="2" t="inlineStr">
         <is>
-          <t>soybeans</t>
+          <t>chia</t>
         </is>
       </c>
       <c r="C188" s="2" t="inlineStr"/>
@@ -2900,7 +2900,7 @@
       <c r="A189" s="2" t="n"/>
       <c r="B189" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">mustard </t>
+          <t>flaxseed</t>
         </is>
       </c>
       <c r="C189" s="2" t="inlineStr"/>
@@ -2912,7 +2912,7 @@
       <c r="A190" s="2" t="n"/>
       <c r="B190" s="2" t="inlineStr">
         <is>
-          <t>sunflower</t>
+          <t xml:space="preserve">mustard </t>
         </is>
       </c>
       <c r="C190" s="2" t="inlineStr"/>
@@ -2924,7 +2924,7 @@
       <c r="A191" s="2" t="n"/>
       <c r="B191" s="2" t="inlineStr">
         <is>
-          <t>chia</t>
+          <t>peanuts</t>
         </is>
       </c>
       <c r="C191" s="2" t="inlineStr"/>
@@ -2960,7 +2960,7 @@
       <c r="A194" s="2" t="n"/>
       <c r="B194" s="2" t="inlineStr">
         <is>
-          <t>peanuts</t>
+          <t>soybeans</t>
         </is>
       </c>
       <c r="C194" s="2" t="inlineStr"/>
@@ -2972,7 +2972,7 @@
       <c r="A195" s="2" t="n"/>
       <c r="B195" s="2" t="inlineStr">
         <is>
-          <t>flaxseed</t>
+          <t>sunflower</t>
         </is>
       </c>
       <c r="C195" s="2" t="inlineStr"/>
@@ -2988,7 +2988,7 @@
       </c>
       <c r="B196" s="2" t="inlineStr">
         <is>
-          <t>yarrow</t>
+          <t>clover</t>
         </is>
       </c>
       <c r="C196" s="2" t="inlineStr"/>
@@ -3000,7 +3000,7 @@
       <c r="A197" s="2" t="n"/>
       <c r="B197" s="2" t="inlineStr">
         <is>
-          <t>sorghum forage</t>
+          <t>lucerne</t>
         </is>
       </c>
       <c r="C197" s="2" t="inlineStr"/>
@@ -3012,7 +3012,7 @@
       <c r="A198" s="2" t="n"/>
       <c r="B198" s="2" t="inlineStr">
         <is>
-          <t>turnips forage</t>
+          <t>plantain</t>
         </is>
       </c>
       <c r="C198" s="2" t="inlineStr"/>
@@ -3024,7 +3024,7 @@
       <c r="A199" s="2" t="n"/>
       <c r="B199" s="2" t="inlineStr">
         <is>
-          <t>lucerne</t>
+          <t>sorghum forage</t>
         </is>
       </c>
       <c r="C199" s="2" t="inlineStr"/>
@@ -3036,7 +3036,7 @@
       <c r="A200" s="2" t="n"/>
       <c r="B200" s="2" t="inlineStr">
         <is>
-          <t>plantain</t>
+          <t>turnips forage</t>
         </is>
       </c>
       <c r="C200" s="2" t="inlineStr"/>
@@ -3048,7 +3048,7 @@
       <c r="A201" s="2" t="n"/>
       <c r="B201" s="2" t="inlineStr">
         <is>
-          <t>clover</t>
+          <t>yarrow</t>
         </is>
       </c>
       <c r="C201" s="2" t="inlineStr"/>
@@ -3062,11 +3062,7 @@
           <t>Pulses</t>
         </is>
       </c>
-      <c r="B202" s="2" t="inlineStr">
-        <is>
-          <t>navy bean</t>
-        </is>
-      </c>
+      <c r="B202" s="2" t="inlineStr"/>
       <c r="C202" s="2" t="inlineStr"/>
       <c r="D202" s="2" t="inlineStr"/>
       <c r="E202" s="2" t="inlineStr"/>
@@ -3088,7 +3084,7 @@
       <c r="A204" s="2" t="n"/>
       <c r="B204" s="2" t="inlineStr">
         <is>
-          <t>lupins</t>
+          <t>broad beans</t>
         </is>
       </c>
       <c r="C204" s="2" t="inlineStr"/>
@@ -3100,7 +3096,7 @@
       <c r="A205" s="2" t="n"/>
       <c r="B205" s="2" t="inlineStr">
         <is>
-          <t>vetches</t>
+          <t>chickpeas</t>
         </is>
       </c>
       <c r="C205" s="2" t="inlineStr"/>
@@ -3112,7 +3108,7 @@
       <c r="A206" s="2" t="n"/>
       <c r="B206" s="2" t="inlineStr">
         <is>
-          <t>field beans</t>
+          <t>cowpea</t>
         </is>
       </c>
       <c r="C206" s="2" t="inlineStr"/>
@@ -3124,7 +3120,7 @@
       <c r="A207" s="2" t="n"/>
       <c r="B207" s="2" t="inlineStr">
         <is>
-          <t>lentils</t>
+          <t>field beans</t>
         </is>
       </c>
       <c r="C207" s="2" t="inlineStr"/>
@@ -3134,7 +3130,11 @@
     </row>
     <row r="208">
       <c r="A208" s="2" t="n"/>
-      <c r="B208" s="2" t="inlineStr"/>
+      <c r="B208" s="2" t="inlineStr">
+        <is>
+          <t>field peas</t>
+        </is>
+      </c>
       <c r="C208" s="2" t="inlineStr"/>
       <c r="D208" s="2" t="inlineStr"/>
       <c r="E208" s="2" t="inlineStr"/>
@@ -3144,7 +3144,7 @@
       <c r="A209" s="2" t="n"/>
       <c r="B209" s="2" t="inlineStr">
         <is>
-          <t>broad beans</t>
+          <t>lentils</t>
         </is>
       </c>
       <c r="C209" s="2" t="inlineStr"/>
@@ -3156,7 +3156,7 @@
       <c r="A210" s="2" t="n"/>
       <c r="B210" s="2" t="inlineStr">
         <is>
-          <t>chickpeas</t>
+          <t>lupins</t>
         </is>
       </c>
       <c r="C210" s="2" t="inlineStr"/>
@@ -3168,7 +3168,7 @@
       <c r="A211" s="2" t="n"/>
       <c r="B211" s="2" t="inlineStr">
         <is>
-          <t>cowpea</t>
+          <t>navy bean</t>
         </is>
       </c>
       <c r="C211" s="2" t="inlineStr"/>
@@ -3192,7 +3192,7 @@
       <c r="A213" s="2" t="n"/>
       <c r="B213" s="2" t="inlineStr">
         <is>
-          <t>field peas</t>
+          <t>vetches</t>
         </is>
       </c>
       <c r="C213" s="2" t="inlineStr"/>
@@ -3208,7 +3208,7 @@
       </c>
       <c r="B214" s="2" t="inlineStr">
         <is>
-          <t>eggplants</t>
+          <t>arrowroot</t>
         </is>
       </c>
       <c r="C214" s="2" t="inlineStr"/>
@@ -3220,7 +3220,7 @@
       <c r="A215" s="2" t="n"/>
       <c r="B215" s="2" t="inlineStr">
         <is>
-          <t>carrots</t>
+          <t>artichokes</t>
         </is>
       </c>
       <c r="C215" s="2" t="inlineStr"/>
@@ -3232,7 +3232,7 @@
       <c r="A216" s="2" t="n"/>
       <c r="B216" s="2" t="inlineStr">
         <is>
-          <t>arrowroot</t>
+          <t>asparagus</t>
         </is>
       </c>
       <c r="C216" s="2" t="inlineStr"/>
@@ -3244,7 +3244,7 @@
       <c r="A217" s="2" t="n"/>
       <c r="B217" s="2" t="inlineStr">
         <is>
-          <t>pumpkins</t>
+          <t>beans</t>
         </is>
       </c>
       <c r="C217" s="2" t="inlineStr"/>
@@ -3256,7 +3256,7 @@
       <c r="A218" s="2" t="n"/>
       <c r="B218" s="2" t="inlineStr">
         <is>
-          <t>rocket</t>
+          <t>beetroot</t>
         </is>
       </c>
       <c r="C218" s="2" t="inlineStr"/>
@@ -3268,7 +3268,7 @@
       <c r="A219" s="2" t="n"/>
       <c r="B219" s="2" t="inlineStr">
         <is>
-          <t>burdock</t>
+          <t>bitter melon</t>
         </is>
       </c>
       <c r="C219" s="2" t="inlineStr"/>
@@ -3280,7 +3280,7 @@
       <c r="A220" s="2" t="n"/>
       <c r="B220" s="2" t="inlineStr">
         <is>
-          <t>sweet corn</t>
+          <t>broccoli</t>
         </is>
       </c>
       <c r="C220" s="2" t="inlineStr"/>
@@ -3292,7 +3292,7 @@
       <c r="A221" s="2" t="n"/>
       <c r="B221" s="2" t="inlineStr">
         <is>
-          <t>radishes</t>
+          <t>brussels sprouts</t>
         </is>
       </c>
       <c r="C221" s="2" t="inlineStr"/>
@@ -3304,7 +3304,7 @@
       <c r="A222" s="2" t="n"/>
       <c r="B222" s="2" t="inlineStr">
         <is>
-          <t>sage</t>
+          <t>burdock</t>
         </is>
       </c>
       <c r="C222" s="2" t="inlineStr"/>
@@ -3316,7 +3316,7 @@
       <c r="A223" s="2" t="n"/>
       <c r="B223" s="2" t="inlineStr">
         <is>
-          <t>chicory</t>
+          <t>cabbages</t>
         </is>
       </c>
       <c r="C223" s="2" t="inlineStr"/>
@@ -3328,7 +3328,7 @@
       <c r="A224" s="2" t="n"/>
       <c r="B224" s="2" t="inlineStr">
         <is>
-          <t>rosemary</t>
+          <t>capsicums</t>
         </is>
       </c>
       <c r="C224" s="2" t="inlineStr"/>
@@ -3340,7 +3340,7 @@
       <c r="A225" s="2" t="n"/>
       <c r="B225" s="2" t="inlineStr">
         <is>
-          <t>marjoram</t>
+          <t>carrots</t>
         </is>
       </c>
       <c r="C225" s="2" t="inlineStr"/>
@@ -3352,7 +3352,7 @@
       <c r="A226" s="2" t="n"/>
       <c r="B226" s="2" t="inlineStr">
         <is>
-          <t>parsnips</t>
+          <t>cauliflowers</t>
         </is>
       </c>
       <c r="C226" s="2" t="inlineStr"/>
@@ -3364,7 +3364,7 @@
       <c r="A227" s="2" t="n"/>
       <c r="B227" s="2" t="inlineStr">
         <is>
-          <t>chives</t>
+          <t>celery</t>
         </is>
       </c>
       <c r="C227" s="2" t="inlineStr"/>
@@ -3376,7 +3376,7 @@
       <c r="A228" s="2" t="n"/>
       <c r="B228" s="2" t="inlineStr">
         <is>
-          <t>okra</t>
+          <t>chamomile</t>
         </is>
       </c>
       <c r="C228" s="2" t="inlineStr"/>
@@ -3388,7 +3388,7 @@
       <c r="A229" s="2" t="n"/>
       <c r="B229" s="2" t="inlineStr">
         <is>
-          <t>artichokes</t>
+          <t>chervil</t>
         </is>
       </c>
       <c r="C229" s="2" t="inlineStr"/>
@@ -3400,7 +3400,7 @@
       <c r="A230" s="2" t="n"/>
       <c r="B230" s="2" t="inlineStr">
         <is>
-          <t>broccoli</t>
+          <t>chicory</t>
         </is>
       </c>
       <c r="C230" s="2" t="inlineStr"/>
@@ -3412,7 +3412,7 @@
       <c r="A231" s="2" t="n"/>
       <c r="B231" s="2" t="inlineStr">
         <is>
-          <t>cauliflowers</t>
+          <t>chillies</t>
         </is>
       </c>
       <c r="C231" s="2" t="inlineStr"/>
@@ -3424,7 +3424,7 @@
       <c r="A232" s="2" t="n"/>
       <c r="B232" s="2" t="inlineStr">
         <is>
-          <t>cucumbers</t>
+          <t>chinese cabbages</t>
         </is>
       </c>
       <c r="C232" s="2" t="inlineStr"/>
@@ -3436,7 +3436,7 @@
       <c r="A233" s="2" t="n"/>
       <c r="B233" s="2" t="inlineStr">
         <is>
-          <t>kale</t>
+          <t>chives</t>
         </is>
       </c>
       <c r="C233" s="2" t="inlineStr"/>
@@ -3448,7 +3448,7 @@
       <c r="A234" s="2" t="n"/>
       <c r="B234" s="2" t="inlineStr">
         <is>
-          <t>thyme</t>
+          <t>coriander</t>
         </is>
       </c>
       <c r="C234" s="2" t="inlineStr"/>
@@ -3460,7 +3460,7 @@
       <c r="A235" s="2" t="n"/>
       <c r="B235" s="2" t="inlineStr">
         <is>
-          <t>celery</t>
+          <t>cucumbers</t>
         </is>
       </c>
       <c r="C235" s="2" t="inlineStr"/>
@@ -3472,7 +3472,7 @@
       <c r="A236" s="2" t="n"/>
       <c r="B236" s="2" t="inlineStr">
         <is>
-          <t>onions</t>
+          <t>echinacea</t>
         </is>
       </c>
       <c r="C236" s="2" t="inlineStr"/>
@@ -3484,7 +3484,7 @@
       <c r="A237" s="2" t="n"/>
       <c r="B237" s="2" t="inlineStr">
         <is>
-          <t>turnips</t>
+          <t>eggplants</t>
         </is>
       </c>
       <c r="C237" s="2" t="inlineStr"/>
@@ -3496,7 +3496,7 @@
       <c r="A238" s="2" t="n"/>
       <c r="B238" s="2" t="inlineStr">
         <is>
-          <t>lettuces</t>
+          <t>fennel</t>
         </is>
       </c>
       <c r="C238" s="2" t="inlineStr"/>
@@ -3508,7 +3508,7 @@
       <c r="A239" s="2" t="n"/>
       <c r="B239" s="2" t="inlineStr">
         <is>
-          <t>peas</t>
+          <t>french beans</t>
         </is>
       </c>
       <c r="C239" s="2" t="inlineStr"/>
@@ -3520,7 +3520,7 @@
       <c r="A240" s="2" t="n"/>
       <c r="B240" s="2" t="inlineStr">
         <is>
-          <t>swedes</t>
+          <t>garlic</t>
         </is>
       </c>
       <c r="C240" s="2" t="inlineStr"/>
@@ -3532,7 +3532,7 @@
       <c r="A241" s="2" t="n"/>
       <c r="B241" s="2" t="inlineStr">
         <is>
-          <t>cabbages</t>
+          <t>gherkins</t>
         </is>
       </c>
       <c r="C241" s="2" t="inlineStr"/>
@@ -3544,7 +3544,7 @@
       <c r="A242" s="2" t="n"/>
       <c r="B242" s="2" t="inlineStr">
         <is>
-          <t>kumara</t>
+          <t>herbs</t>
         </is>
       </c>
       <c r="C242" s="2" t="inlineStr"/>
@@ -3556,7 +3556,7 @@
       <c r="A243" s="2" t="n"/>
       <c r="B243" s="2" t="inlineStr">
         <is>
-          <t>echinacea</t>
+          <t>kale</t>
         </is>
       </c>
       <c r="C243" s="2" t="inlineStr"/>
@@ -3568,7 +3568,7 @@
       <c r="A244" s="2" t="n"/>
       <c r="B244" s="2" t="inlineStr">
         <is>
-          <t>oregano</t>
+          <t>kumara</t>
         </is>
       </c>
       <c r="C244" s="2" t="inlineStr"/>
@@ -3580,7 +3580,7 @@
       <c r="A245" s="2" t="n"/>
       <c r="B245" s="2" t="inlineStr">
         <is>
-          <t>sugar beet</t>
+          <t>leeks</t>
         </is>
       </c>
       <c r="C245" s="2" t="inlineStr"/>
@@ -3592,7 +3592,7 @@
       <c r="A246" s="2" t="n"/>
       <c r="B246" s="2" t="inlineStr">
         <is>
-          <t>capsicums</t>
+          <t>lemongrass</t>
         </is>
       </c>
       <c r="C246" s="2" t="inlineStr"/>
@@ -3604,7 +3604,7 @@
       <c r="A247" s="2" t="n"/>
       <c r="B247" s="2" t="inlineStr">
         <is>
-          <t>chillies</t>
+          <t>lettuces</t>
         </is>
       </c>
       <c r="C247" s="2" t="inlineStr"/>
@@ -3616,7 +3616,7 @@
       <c r="A248" s="2" t="n"/>
       <c r="B248" s="2" t="inlineStr">
         <is>
-          <t>truffles</t>
+          <t>marjoram</t>
         </is>
       </c>
       <c r="C248" s="2" t="inlineStr"/>
@@ -3628,7 +3628,7 @@
       <c r="A249" s="2" t="n"/>
       <c r="B249" s="2" t="inlineStr">
         <is>
-          <t>silverbeet and spinach</t>
+          <t>marrows and squashes</t>
         </is>
       </c>
       <c r="C249" s="2" t="inlineStr"/>
@@ -3640,7 +3640,7 @@
       <c r="A250" s="2" t="n"/>
       <c r="B250" s="2" t="inlineStr">
         <is>
-          <t>french beans</t>
+          <t>mint</t>
         </is>
       </c>
       <c r="C250" s="2" t="inlineStr"/>
@@ -3652,7 +3652,7 @@
       <c r="A251" s="2" t="n"/>
       <c r="B251" s="2" t="inlineStr">
         <is>
-          <t>sweet potatoes</t>
+          <t>mushrooms</t>
         </is>
       </c>
       <c r="C251" s="2" t="inlineStr"/>
@@ -3664,7 +3664,7 @@
       <c r="A252" s="2" t="n"/>
       <c r="B252" s="2" t="inlineStr">
         <is>
-          <t>tomatoes</t>
+          <t>okra</t>
         </is>
       </c>
       <c r="C252" s="2" t="inlineStr"/>
@@ -3676,7 +3676,7 @@
       <c r="A253" s="2" t="n"/>
       <c r="B253" s="2" t="inlineStr">
         <is>
-          <t>rhubarb</t>
+          <t>onions</t>
         </is>
       </c>
       <c r="C253" s="2" t="inlineStr"/>
@@ -3688,7 +3688,7 @@
       <c r="A254" s="2" t="n"/>
       <c r="B254" s="2" t="inlineStr">
         <is>
-          <t>vegetables</t>
+          <t>oregano</t>
         </is>
       </c>
       <c r="C254" s="2" t="inlineStr"/>
@@ -3700,7 +3700,7 @@
       <c r="A255" s="2" t="n"/>
       <c r="B255" s="2" t="inlineStr">
         <is>
-          <t>snowpeas</t>
+          <t>parsley</t>
         </is>
       </c>
       <c r="C255" s="2" t="inlineStr"/>
@@ -3712,7 +3712,7 @@
       <c r="A256" s="2" t="n"/>
       <c r="B256" s="2" t="inlineStr">
         <is>
-          <t>coriander</t>
+          <t>parsnips</t>
         </is>
       </c>
       <c r="C256" s="2" t="inlineStr"/>
@@ -3724,7 +3724,7 @@
       <c r="A257" s="2" t="n"/>
       <c r="B257" s="2" t="inlineStr">
         <is>
-          <t>tarragon</t>
+          <t>peas</t>
         </is>
       </c>
       <c r="C257" s="2" t="inlineStr"/>
@@ -3736,7 +3736,7 @@
       <c r="A258" s="2" t="n"/>
       <c r="B258" s="2" t="inlineStr">
         <is>
-          <t>zucchini</t>
+          <t>peppermint</t>
         </is>
       </c>
       <c r="C258" s="2" t="inlineStr"/>
@@ -3748,7 +3748,7 @@
       <c r="A259" s="2" t="n"/>
       <c r="B259" s="2" t="inlineStr">
         <is>
-          <t>herbs</t>
+          <t>potatoes</t>
         </is>
       </c>
       <c r="C259" s="2" t="inlineStr"/>
@@ -3760,7 +3760,7 @@
       <c r="A260" s="2" t="n"/>
       <c r="B260" s="2" t="inlineStr">
         <is>
-          <t>mushrooms</t>
+          <t>pumpkins</t>
         </is>
       </c>
       <c r="C260" s="2" t="inlineStr"/>
@@ -3772,7 +3772,7 @@
       <c r="A261" s="2" t="n"/>
       <c r="B261" s="2" t="inlineStr">
         <is>
-          <t>gherkins</t>
+          <t>radishes</t>
         </is>
       </c>
       <c r="C261" s="2" t="inlineStr"/>
@@ -3784,7 +3784,7 @@
       <c r="A262" s="2" t="n"/>
       <c r="B262" s="2" t="inlineStr">
         <is>
-          <t>marrows and squashes</t>
+          <t>rhubarb</t>
         </is>
       </c>
       <c r="C262" s="2" t="inlineStr"/>
@@ -3796,7 +3796,7 @@
       <c r="A263" s="2" t="n"/>
       <c r="B263" s="2" t="inlineStr">
         <is>
-          <t>lemongrass</t>
+          <t>rocket</t>
         </is>
       </c>
       <c r="C263" s="2" t="inlineStr"/>
@@ -3808,7 +3808,7 @@
       <c r="A264" s="2" t="n"/>
       <c r="B264" s="2" t="inlineStr">
         <is>
-          <t>potatoes</t>
+          <t>rosemary</t>
         </is>
       </c>
       <c r="C264" s="2" t="inlineStr"/>
@@ -3820,7 +3820,7 @@
       <c r="A265" s="2" t="n"/>
       <c r="B265" s="2" t="inlineStr">
         <is>
-          <t>spring onions and shallots</t>
+          <t>sage</t>
         </is>
       </c>
       <c r="C265" s="2" t="inlineStr"/>
@@ -3832,7 +3832,7 @@
       <c r="A266" s="2" t="n"/>
       <c r="B266" s="2" t="inlineStr">
         <is>
-          <t>leeks</t>
+          <t>silverbeet and spinach</t>
         </is>
       </c>
       <c r="C266" s="2" t="inlineStr"/>
@@ -3844,7 +3844,7 @@
       <c r="A267" s="2" t="n"/>
       <c r="B267" s="2" t="inlineStr">
         <is>
-          <t>beetroot</t>
+          <t>snowpeas</t>
         </is>
       </c>
       <c r="C267" s="2" t="inlineStr"/>
@@ -3856,7 +3856,7 @@
       <c r="A268" s="2" t="n"/>
       <c r="B268" s="2" t="inlineStr">
         <is>
-          <t>asparagus</t>
+          <t>spring onions and shallots</t>
         </is>
       </c>
       <c r="C268" s="2" t="inlineStr"/>
@@ -3868,7 +3868,7 @@
       <c r="A269" s="2" t="n"/>
       <c r="B269" s="2" t="inlineStr">
         <is>
-          <t>bitter melon</t>
+          <t>sprouts</t>
         </is>
       </c>
       <c r="C269" s="2" t="inlineStr"/>
@@ -3880,7 +3880,7 @@
       <c r="A270" s="2" t="n"/>
       <c r="B270" s="2" t="inlineStr">
         <is>
-          <t>garlic</t>
+          <t>sugar beet</t>
         </is>
       </c>
       <c r="C270" s="2" t="inlineStr"/>
@@ -3892,7 +3892,7 @@
       <c r="A271" s="2" t="n"/>
       <c r="B271" s="2" t="inlineStr">
         <is>
-          <t>peppermint</t>
+          <t>swedes</t>
         </is>
       </c>
       <c r="C271" s="2" t="inlineStr"/>
@@ -3904,7 +3904,7 @@
       <c r="A272" s="2" t="n"/>
       <c r="B272" s="2" t="inlineStr">
         <is>
-          <t>mint</t>
+          <t>sweet corn</t>
         </is>
       </c>
       <c r="C272" s="2" t="inlineStr"/>
@@ -3916,7 +3916,7 @@
       <c r="A273" s="2" t="n"/>
       <c r="B273" s="2" t="inlineStr">
         <is>
-          <t>vegetable seeds</t>
+          <t>sweet potatoes</t>
         </is>
       </c>
       <c r="C273" s="2" t="inlineStr"/>
@@ -3928,7 +3928,7 @@
       <c r="A274" s="2" t="n"/>
       <c r="B274" s="2" t="inlineStr">
         <is>
-          <t>sprouts</t>
+          <t>tarragon</t>
         </is>
       </c>
       <c r="C274" s="2" t="inlineStr"/>
@@ -3940,7 +3940,7 @@
       <c r="A275" s="2" t="n"/>
       <c r="B275" s="2" t="inlineStr">
         <is>
-          <t>parsley</t>
+          <t>thyme</t>
         </is>
       </c>
       <c r="C275" s="2" t="inlineStr"/>
@@ -3952,7 +3952,7 @@
       <c r="A276" s="2" t="n"/>
       <c r="B276" s="2" t="inlineStr">
         <is>
-          <t>chamomile</t>
+          <t>tomatoes</t>
         </is>
       </c>
       <c r="C276" s="2" t="inlineStr"/>
@@ -3964,7 +3964,7 @@
       <c r="A277" s="2" t="n"/>
       <c r="B277" s="2" t="inlineStr">
         <is>
-          <t>fennel</t>
+          <t>truffles</t>
         </is>
       </c>
       <c r="C277" s="2" t="inlineStr"/>
@@ -3976,7 +3976,7 @@
       <c r="A278" s="2" t="n"/>
       <c r="B278" s="2" t="inlineStr">
         <is>
-          <t>beans</t>
+          <t>turnips</t>
         </is>
       </c>
       <c r="C278" s="2" t="inlineStr"/>
@@ -3988,7 +3988,7 @@
       <c r="A279" s="2" t="n"/>
       <c r="B279" s="2" t="inlineStr">
         <is>
-          <t>chinese cabbages</t>
+          <t>vegetable seeds</t>
         </is>
       </c>
       <c r="C279" s="2" t="inlineStr"/>
@@ -4000,7 +4000,7 @@
       <c r="A280" s="2" t="n"/>
       <c r="B280" s="2" t="inlineStr">
         <is>
-          <t>brussels sprouts</t>
+          <t>vegetables</t>
         </is>
       </c>
       <c r="C280" s="2" t="inlineStr"/>
@@ -4012,7 +4012,7 @@
       <c r="A281" s="2" t="n"/>
       <c r="B281" s="2" t="inlineStr">
         <is>
-          <t>chervil</t>
+          <t>zucchini</t>
         </is>
       </c>
       <c r="C281" s="2" t="inlineStr"/>

</xml_diff>